<commit_message>
se realizo algunas modificaciones el los spyders
</commit_message>
<xml_diff>
--- a/data/27-03-22/data_transform.xlsx
+++ b/data/27-03-22/data_transform.xlsx
@@ -498,17 +498,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>rally vuelta a marbán aprehenden a corredor que atropelló a un menor</t>
+          <t>ucrania y rusia retoman diálogo en turquía</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> el motociclista que atropelló a un menor de edad en el rally vuelta a marbán fue aprehendido informó el director de tránsito del beni coronel marcos céspedes el conductor fue identificado como antonio chemo cuellar de 33 años de edad arrolló al menor la tarde de este domingo cuando cruzaba la ruta del rally en la población de sachojere la competencia fue organizada por novena vez por la asociación beniana de motociclismo y sus representantes aseguraron que están al pendiente del estado de salud tanto del menor como del motociclista céspedes detalló que el conductor sufrió un tec leve y fractura de falange de tercer grado en la mano derecha y está internado en una clínica privada reportó la red erbol “él chemo también se encuentra internado pero además se encuentra aprehendido por disposición del ministerio público” señaló el diagnóstico del menor es reservado sin embargo se conoce que fue intervenido quirúrgicamente en el hospital obrero sufrió un fuerte golpe en la cabeza y tiene una de sus piernas fracturadas el caso fue clasificado por la dirección de tránsito como atropello a peatón en competencia deportiva “sí se debe investigar porque hay lesiones gravísimas o graves y obviamente en el transcurso de la investigación se van a determinar las situaciones que se vayan a seguir posteriormente no porque nosotros hayamos visto que no hay responsabilidad se va a dejar de investigar se tiene que investigar y si el caso amerita obviamente se va a archivar y se va a rechazar” manifestó el coronel /jdlf/</t>
+          <t xml:space="preserve"> tras varios intentos fallidos ambas naciones pactaron una nueva ronda de diálogo para la siguiente semana los puntos clave de las negociaciones siguen siendo la inclusión de ucrania a la organización del tratado del atlántico norte otan su posterior desarme y el estatus de crimea delegados de ucrania y rusia tienen previsto reunirse de nuevo en el transcurso de esta semana de manera presencial el escenario de las negociaciones será turquía según lo anunciado por ambas delegaciones los presidentes de turquía recep tayyip erdogan y de rusia vladimir putin acordaron celebrar la siguiente ronda de negociaciones entre las delegaciones rusa y ucraniana en estambul declaró la presidencia turca en un comunicado erdogan le aseguró a putin que turquía estaba dispuesta a hacer las contribuciones necesarias para establecer un alto el fuego en ucrania y mejorar la condición humanitaria en la región “durante las discusiones por videoconferencia de hoy se decidió celebrar la próxima ronda cara a cara en turquía del 28 al 30 de marzo” dijo el negociador ucraniano david arakhamia citado por la agencia de noticias afp en cambio el jefe de los negociadores rusos vladimir medinsky confirmó que habrá una nueva ronda de conversaciones pero dijo que se realizarán el martes y el miércoles aunque no precisó dónde las conversaciones entre ambas delegaciones comenzaron el 28 de febrero apenas cuatro días después del inicio de las operaciones militares el primer encuentro fue en bielorrusia en lo que acordaron entre otras cosas la apertura de corredores humanitarios para evacuar civiles posteriormente el 10 de marzo los cancilleres de ucrania y rusia dmytro kuleba y serguei lavrov se encontraron en antalya turquía junto a su par turco mevlut cavusoglu hasta ahora ese fue el único contacto directo entre los cancilleres de las dos partes del conflicto entre los seis puntos en debate figuran la renuncia de ucrania a su deseo de incorporarse a la otan y el desarme de ese país además de las garantías de seguridad recíprocas con rusia las delegaciones también discutieron sobre el reclamo de rusia para la eliminación de elementos ultranacionalistas en el gobierno de kiev lo que moscú llama “desnazificación” y el levantamiento de las restricciones sobre el uso del idioma ruso en ucrania / lmpt</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/21/rally-vuelta-a-marban-aprehenden-a-corredor-que-atropello-a-un-menor/</t>
+          <t>https://lapatria.bo/2022/03/27/ucrania-y-rusia-retoman-dialogo-en-turquia/</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -518,51 +518,51 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>38627075644f3e58c9cf8ae402d5652e</t>
+          <t>94c517935cc52f852a23404f7c0d11b6</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="G2" t="n">
-        <v>1524</v>
+        <v>2299</v>
       </c>
       <c r="H2" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I2" t="n">
-        <v>134</v>
+        <v>211</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>('menor', 4)</t>
+          <t>('ucrania', 6)</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>('investigar', 3)</t>
+          <t>('rusia', 5)</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>('motociclista', 2)</t>
+          <t>('turquía', 5)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>policía aprehende a vladimir irahola villanueva presunto feminicida de vania</t>
+          <t>gobierno peruano pide a la oea presenciar debate de moción de vacancia de pedro castillo</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> la policía informó que luego de un trabajo investigativo en poblaciones fronterizas del beni se ha logrado aprehender a vladimir irahola villanueva principal acusado del feminicidio de su pareja vania trujillo crimen ocurrido en febrero en la ciudad de la paz “informamos a la población que después de un arduo trabajo investigativo en poblaciones fronterizas del beni nuestros servidores policiales procedieron a la aprehensión de vladimir irahola villanueva principal acusado del feminicidio de su esposa vania trujillo” se lee en el comunicado de la policía en sus redes sociales el caso cobró relevancia después de que la activista maría galindo protestó en el estado mayor y la fiscalía reclamando que se había dejado escapar a vladimir irahola presunto autor del feminicidio de vania trujillo el feminicidio se registró el 18 de febrero según las investigaciones el autor del crimen quiso fingir que la víctima había fallecido por ingerir una sustancia tóxica pero se evidenció que fue estrangulada el padre del presunto feminicida de profesión militar fue aprehendido y enviado a la cárcel acusado de haber ayudado a escapar a su hijo con el pasar de los días las investigaciones se volcaron al beni donde vive un amigo del principal sospechoso quien aparentemente sabía del crimen y cobijó al presunto feminicida por lo cual fue aprehendido vladimir irahola se comunicó con su amigo moisés quien se encontraba en beni y le contó que le quitó la vida a su pareja el amigo le pidió fotos y ambos se enviaron audios “por eso que se llega a estas conversaciones y se tiene la aprehensión de moisés vaquero que sería el amigo a quien denominaba ‘yunta o bro’” afirmo la coordinadora de la fiscalía de la paz nilda calle vania trujillo fue asesinada el 18 de febrero en la zona de bajo san antonio de la ciudad de la paz presuntamente en manos de su concubino vladimir de quien se presume que le puso en la boca un líquido usado para limpiar hornos y de esa forma hacer creer que la joven se suicidó sin embargo tras la autopsia se develó que el deceso fue por estrangulamiento /hnf/</t>
+          <t xml:space="preserve"> desde el gobierno peruano solicitaron la jornada precedente la presencia de funcionarios de la organización de los estados americanos oea para presenciar el debate de moción de vacancia del presidente pedro castillo el congreso escuchará el 28 de marzo la defensa del mandatario para tratar el tema de su destitución en una misiva enviada por el canciller césar landa a la presidenta del congreso maría carmen alva se solicitó que se acepte la presencia de testigos de la oea con el motivo de que el debate se desarrolle con trasparencia ante la ciudadanía y la comunidad internacional en la carta se expresó la importancia de este acontecimiento pues para landa depende de este proceso la gobernabilidad de perú y la vigencia de la democracia no solo en ese país sino en todo el continente el canciller pidió la presencia de tres funcionarios específicos de la oea para que presencien el debate en el pleno del congreso el representante de ese ente en el perú miguel ángel trinidad el secretario de asuntos jurídicos jean miguel arrighi y la secretaria de acceso a derechos y equidad maricarmen plata el partido opositor “avanza país” cuestionó esta petición a la presidencia del congreso pues consideraron que no hay precedentes para incluir a la oea como veedores en un proceso como la vacancia según informó el portal de noticias deutsche welle por su parte el primer ministro aníbal torres destacó el pronunciamiento de la comisión interamericana de derechos humanos cidh quienes expresaron el viernes reciente su preocupación por la situación política en perú y el impacto que podría tener en los derechos humanos «la vacancia presidencial debe llevarse a cabo conforme al debido proceso constitucional y fundarse en conductas señaladas con precisión que doten a este proceso de objetividad imparcialidad y garantías del debido proceso a fin de asegurar que sea un recurso que no se use para afectar el orden democrático constituido y los derechos políticos de los y las peruanas» informó la comisión en un comunicado el lunes 28 de marzo el congreso escuchará la defensa de pedro castillo ante la acusación por una supuesta «incapacidad moral permanente» posteriormente se votará el pedido de destitución presentado por varios grupos de ultraderecha que aparentemente no cuentan con los 87 votos necesarios para hacer a abandonar el cargo al presidente / lmpt</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/23/policia-aprehende-a-vladimir-irahola-villanueva-presunto-feminicida-de-vania/</t>
+          <t>https://lapatria.bo/2022/03/26/gobierno-peruano-pide-a-la-oea-presenciar-debate-de-mocion-de-vacancia-de-pedro-castillo/</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -572,51 +572,51 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>57e927df02d32b98814406604e0e832f</t>
+          <t>4c8b311107f359a09f787328ed22add5</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="G3" t="n">
-        <v>2086</v>
+        <v>2367</v>
       </c>
       <c r="H3" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I3" t="n">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>('vladimir', 5)</t>
+          <t>('congreso', 5)</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>('beni', 4)</t>
+          <t>('proceso', 5)</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>('irahola', 4)</t>
+          <t>('oea', 4)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ucrania y rusia retoman diálogo en turquía</t>
+          <t>el salvador declara estado de excepción ante la escalada criminal</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> tras varios intentos fallidos ambas naciones pactaron una nueva ronda de diálogo para la siguiente semana los puntos clave de las negociaciones siguen siendo la inclusión de ucrania a la organización del tratado del atlántico norte otan su posterior desarme y el estatus de crimea delegados de ucrania y rusia tienen previsto reunirse de nuevo en el transcurso de esta semana de manera presencial el escenario de las negociaciones será turquía según lo anunciado por ambas delegaciones los presidentes de turquía recep tayyip erdogan y de rusia vladimir putin acordaron celebrar la siguiente ronda de negociaciones entre las delegaciones rusa y ucraniana en estambul declaró la presidencia turca en un comunicado erdogan le aseguró a putin que turquía estaba dispuesta a hacer las contribuciones necesarias para establecer un alto el fuego en ucrania y mejorar la condición humanitaria en la región “durante las discusiones por videoconferencia de hoy se decidió celebrar la próxima ronda cara a cara en turquía del 28 al 30 de marzo” dijo el negociador ucraniano david arakhamia citado por la agencia de noticias afp en cambio el jefe de los negociadores rusos vladimir medinsky confirmó que habrá una nueva ronda de conversaciones pero dijo que se realizarán el martes y el miércoles aunque no precisó dónde las conversaciones entre ambas delegaciones comenzaron el 28 de febrero apenas cuatro días después del inicio de las operaciones militares el primer encuentro fue en bielorrusia en lo que acordaron entre otras cosas la apertura de corredores humanitarios para evacuar civiles posteriormente el 10 de marzo los cancilleres de ucrania y rusia dmytro kuleba y serguei lavrov se encontraron en antalya turquía junto a su par turco mevlut cavusoglu hasta ahora ese fue el único contacto directo entre los cancilleres de las dos partes del conflicto entre los seis puntos en debate figuran la renuncia de ucrania a su deseo de incorporarse a la otan y el desarme de ese país además de las garantías de seguridad recíprocas con rusia las delegaciones también discutieron sobre el reclamo de rusia para la eliminación de elementos ultranacionalistas en el gobierno de kiev lo que moscú llama “desnazificación” y el levantamiento de las restricciones sobre el uso del idioma ruso en ucrania / lmpt</t>
+          <t xml:space="preserve"> la asamblea legislativa de el salvador decretó la madrugada de este domingo un régimen de excepción a raíz de un “incremento desmedido” de los homicidios la muerte de 76 personas en dos días un récord en la historia reciente de ese país fueron atribuidas a las pandillas “declárase en todo el territorio nacional régimen de excepción derivado de las graves perturbaciones al orden público por grupos delincuenciales” consignó el decreto aprobado por amplia mayoría en el parlamento el órgano legislativo con 67 votos de los 84 diputados suspendió por 30 días la libertad de asociación derecho de defensa plazo de detención administrativa inviolabilidad de la correspondencia y telecomunicaciones según informó el portal de noticias infobae el gobierno de nayib bukele planteó</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/27/ucrania-y-rusia-retoman-dialogo-en-turquia/</t>
+          <t>https://lapatria.bo/2022/03/27/el-salvador-declara-estado-de-excepcion-ante-la-escalada-criminal/</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -626,51 +626,51 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>94c517935cc52f852a23404f7c0d11b6</t>
+          <t>82d3d677e39b2cf1c78fbdbbcdc84439</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="G4" t="n">
-        <v>2299</v>
+        <v>2226</v>
       </c>
       <c r="H4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I4" t="n">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>('ucrania', 6)</t>
+          <t>('homicidios', 4)</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>('rusia', 5)</t>
+          <t>('orden', 4)</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>('turquía', 5)</t>
+          <t>('libertad', 4)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>cochabamba policía investiga muerte de una niña que llegó al hospital con signos de violencia</t>
+          <t>aduana extiende horario de atención a operadores hasta las 0300 horas en desaguadero</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> este viernes una madre y el padrastro llevaron el cuerpo sin vida de una niña de 1 año y 9 meses a un hospital de la zona sur de cochabamba ambos explicaron que la menor se había caído de una fuente la policía tras evidenciar que la niña tenía signos de violencia de larga data los arrestó a ambos con fines investigativos según información de los medios de comunicación la niña fue llevada al centro de salud de cerro verde cerca de las 0800 horas de hoy el servicio de emergencia realizó el examen correspondiente y no encontró signos vitales por lo que se realizó maniobras de resucitación sin resultados «al no encontrarse signos vitales se le realiza la resucitación cardiopulmonar por parte del médico de turno pero no fue factible porque no tuvimos una respuesta favorable se le diagnosticó un tec grave y sospecha de fractura de base de cráneo» informó la responsable del hospital la médico jaqueline mamani a red uno los médicos encontraron un hematoma a nivel de la cabeza en la región parietal además un ojo que estaba equimótico y edematizado había lesiones en el lado izquierdo y también un edema y equimosis hasta la región mandibular «el padre refiere que la menor se cayó de una altura de más o menos un metro él dijo que se cayó de la fuente y no se despertó al llegar la menor al hospital ya estaba sin signos vitales sin respuesta alguna» afirmó la responsable del hospital al tratarse de una menor de edad el servicio médico comunicó el hecho a la defensoría y a la felcc quienes llegaron al lugar y retiraron el cuerpo según red uno la fiscal departamental de cochabamba nuria gonzales informó que el ministerio público tomó conocimiento del caso y envió personal para los exámenes correspondientes «la menor en el examen físico registra lesiones de data antigua y una posible situación de agresión sexual por lo cual toda actividad investigativa se está desplegando» dijo gonzales el director de la fuerza especial de lucha contra el crimen felcc ronald tapia informó que el cuerpo de la niña presentaba lesiones de data antigua de hace siete u ocho días a nivel del rostro aparentemente por una caída «estamos a la espera de la autopsia el resultado nos ayudará a determinar lo que podría haber pasado con la menor momentáneamente y con fines investigativos tenemos a dos personas arrestadas que es la mamá y el padrastro posteriormente se determinará la situación legal de ambos» argumentó tapia /hnf/</t>
+          <t xml:space="preserve"> el horario de atención a operadores en el sector de desaguadero se extiende hasta las tres de la madrugada del domingo para facilitar la importación y exportación de mercancía en esta ruta y facilitar el flujo vehicular esta determinación se logró gracias a las gestiones realizadas por la presidente ejecutiva de la aduana nacional an karina serrudo miranda juntamente el superintendente nacional de aduanas de perú luis enrique vera castillo las entidades que decidieron sumarse a la ampliación de horario son el servicio nacional de sanidad agropecuaria e inocuidad alimentaria senasag la dirección general de migración la superintendencia nacional de aduanas y de administración tributaria sunat de perú y el centro binacional de atención en frontera cebaf de perú informaron desde la institución aduanera hasta el medio día de la presente jornada la an registró el ingreso de 463 camiones a territorio boliviano con mercancía de exportación en horas de la tarde el proceso de exportación se agilizó un total de 436 camiones de carga ingresaron con normalidad a perú durante las siguientes horas continuarán los turnos para el ingreso y la salida del transporte pesado en la ruta con la finalidad de evitar el congestionamiento y acelerar los procesos tanto de la aduana boliviana como la de su par peruana la an calificó como un éxito las labores logísticas gestionadas pues el descongestionamiento en la carretera desaguadero es evidente en tanto el tránsito de los motorizados de comercio exterior se restableció los resultados de la extensión de horario serán evaluados el domingo de acuerdo a la cantidad de motorizados que continúen a la espera de pasar la frontera entre bolivia y perú con base en ese dato se determinará sí es necesario ampliar la extensión de horario por más días el congestionamiento del flujo vehicular en ese sector se debió a un bloqueo instalado por los comunarios de la provincia ingavi quienes mantuvieron la medida de presión por ocho días continuos exigiendo la construcción de la carretera doble vía río secodesaguadero / lmpt</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/25/cochabamba-policia-investiga-muerte-de-una-nina-que-llego-al-hospital-con-signos-de-violencia/</t>
+          <t>https://lapatria.bo/2022/03/26/aduana-extiende-horario-de-atencion-a-operadores-hasta-las-0300-horas-en-desaguadero/</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -680,51 +680,51 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>5cba75a780eb856f0ecd14d3aecead15</t>
+          <t>abb876b15918cd2a472317f5c1e903a1</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="G5" t="n">
-        <v>2426</v>
+        <v>2067</v>
       </c>
       <c r="H5" t="n">
         <v>9</v>
       </c>
       <c r="I5" t="n">
-        <v>228</v>
+        <v>186</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>('menor', 6)</t>
+          <t>('perú', 5)</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>('niña', 4)</t>
+          <t>('horario', 4)</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>('hospital', 4)</t>
+          <t>('nacional', 4)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>concluyen obras de readecuación en el hospital obrero de la cns</t>
+          <t>covid19 en oruro se detectan dos nuevos casos no se reportan decesos</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> concluyeron las obras de readecuación de ambientes para residencia médica y readecuación e implementación de baños y duchas en el sótano del hospital de atención integral general haig obrero n° 4 el jueves 24 de marzo se realizó la entrega oficial en los ambientes del nosocomio y con la presencia de autoridades de la caja nacional de salud cns tanto nacionales como regionales además de la asistencia de autoridades departamentales se realizó un emotivo acto de entrega de las obras realizadas el administrador regional de la cns johnny bohórquez velasco indicó que las nuevas dependencias tendrán como principales beneficiarios a los residentes médicos tanto actuales como también de futuras generaciones</t>
+          <t xml:space="preserve"> la jornada del 26 de marzo oruro mostró de nuevo una cifra mínima de casos positivos de coronavirus dos en total la tendencia de cero decesos también continuó se cumplieron 18 días sin reportar fallecidos por el virus el reporte del servicio departamental de salud sedes señaló que los dos casos confirmados corresponden al municipio de oruro al igual que las tres personas recuperadas que figuran en el reporte además se descartaron 266 casos total hasta el momento el departamento de oruro registra un total de 35549 casos positivos de coronavirus y 34136 pacientes recuperados actualmente hay 87 casos activos contagios sumados los contagios de la jornada la capital suma 35549 casos positivos de coronavirus seguida huanuni con 1512 casos callapata 1143 machacamarca 392 caracollo 359 sabaya 288 turco 266 salinas de garci mendoza 238 antequera 218 y eucaliptos con 214 casos curahuara de carangas se mantiene con 196 casos al igual que huari con 185 positivos huachacalla 163 santiago de andamarca 154 pazña 149 corque 133 pampa aullagas 103 el choro 87 quillacas 83 en tanto totora 67 huayllamarca 66 soracachi 56 esmeralda 43 yunguyo de litoral 37 belén de andamarca 28 choquecota 26 cruz de machacamarca 26 escara 23 chipaya 21 coipasa 15 la rivera cinco carangas y todos santos uno recuperados ya son 34136 pacientes recuperados en el municipio de oruro huanuni 1469 challapata 1081 machacamarca 374 caracollo 335 sabaya 284 turco 264 salinas de garci mendoza 233 antequera 212 eucaliptus 202 toledo 201 poopó 194 curahuara de carangas se mantiene con 178 pacientes recuperados huari 177 huachacalla 157 santiago de andamarca 148 pazña 146 corque 131 pampa aullagas 101 el choro 87 quillacas 80 huayllamarca 65 finalmente totora 62 soracachi 55 esmeralda 42 yunguyo de litoral 36 belén de andamarca 28 choquecota 25 cruz de machacamarca 24 escara 23 chipaya 21 coipasa 15 la rivera cinco todos santos uno y finalmente carangas uno</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/26/concluyen-obras-de-readecuacion-en-el-hospital-obrero-de-la-cns/</t>
+          <t>https://lapatria.bo/2022/03/26/covid-19-en-oruro-se-detectan-dos-nuevos-casos-no-se-reportan-decesos/</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -734,51 +734,51 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>99786ea273c5645ee5b640ff762c5e73</t>
+          <t>832d0bf674f94b758670c4d51bf045ea</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="G6" t="n">
-        <v>708</v>
+        <v>1940</v>
       </c>
       <c r="H6" t="n">
         <v>6</v>
       </c>
       <c r="I6" t="n">
-        <v>64</v>
+        <v>227</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>('obras', 2)</t>
+          <t>('oruro', 4)</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>('readecuación', 2)</t>
+          <t>('positivos', 4)</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>('ambientes', 2)</t>
+          <t>('recuperados', 4)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>coronavirus seis nuevos casos en oruro y tres pacientes recuperados</t>
+          <t>lima califica como histórico el inicio del juicio contra áñez</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> las cifras de covid19 en oruro continúan bajas después del feriado de carnaval este jueves se tuvieron seis nuevos contagios y tres pacientes recuperados además ya son 16 días que no se reportan decesos por esta enfermedad el reporte del servicio departamental de salud sedes indica que tanto los seis casos nuevos como las tres personas recuperadas son del municipio de oruro total hasta el momento en el departamento de oruro se registraron 42268 casos de coronavirus además 40587 pacientes se recuperaron 1594 fallecieron y hay 87 personas que todavía tienen el virus contagios con los nuevos contagios la ciudad capital suma 35543 casos seguida de huanuni con 1521 challapata 1143 machacamarca 392 caracollo 359 sabaya 288 turco 266 salinas de garci mendoza 238 antequera 218 eucaliptus 214 toledo 210 poopó 209 curahuara de carangas 196 huari 185 huachacalla 163 santiago de andamarca 154 pazña 149 corque 133 pampa aullagas 103 el choro 87 quillacas 83 en tanto totora 67 huayllamarca 66 soracachi 56 esmeralda 43 yunguyo de litoral 37 belén de andamarca 28 choquecota 26 cruz de machacamarca 26 escara 23 chipaya 21 coipasa 15 la rivera cinco carangas y todos santos uno recuperados el municipio de oruro acumula 34130 personas recuperadas huanuni 1469 challapata 1081 machacamarca 374 caracollo 335 sabaya 284 turco 264 salinas de garci mendoza 233 antequera 212 eucaliptus 202 toledo 201 poopó 194 curahuara de carangas 178 huari 177 huachacalla 157 santiago de andamarca 148 pazña 146 corque 131 pampa aullagas 101 el choro 87 quillacas 80 huayllamarca 65 finalmente totora 62 soracachi 55 esmeralda 42 yunguyo de litoral 36 belén de andamarca 28 choquecota 25 cruz de machacamarca 24 escara 23 chipaya 21 coipasa 15 la rivera cinco todos santos uno y carangas uno</t>
+          <t xml:space="preserve"> el ministro de justicia y transparencia institucional iván lima calificó como “histórico” el inicio del juicio denominado golpe de estado ii contra la expresidente jeanine áñez y pidió a su defensa no interferir en el proceso con “chicanas políticas” “mañana es un día histórico esperamos que la defensa de jeanine áñez no obstaculice el debido proceso con ‘chicanas’ que solo afectan al debido proceso y el pedido de #memoriaverdadyjusticia” escribió lima en la cuenta de twitter del ministerio de justicia y transparencia institucional la exmandataria enfrentará un proceso por la vía ordinaria denominado golpe de estado ii que tiene previsto iniciar este jueves 28 en el tribunal 1º de sentencia anticorrupción de la paz el juicio debió iniciarse el 10 de febrero pero fue suspendido ante numerosas objeciones por parte de la acusada según informó el diario la razón pese a que la defensa de jeanine áñez advirtió que presentaría una serie de recursos para que este juicio sea presencial debido a su importancia según lo que argumentaron el proceso será virtual según el nuevo auto de apertura áñez fue acusada por asumir la presidencia del senado en noviembre de 2019 lo que posteriormente le permitió acceder al poder supuestamente sin cumplir el reglamento de debate ni los preceptos constitucionales la defensa legal de la exmandataria negó los cargos y argumentó que todos los procedimientos de sucesión estaban enmarcados en la norma la entonces senadora asumió la presidencia el 12 de noviembre de 2019 después de varios días de disturbios en el país que produjeron posteriormente la renuncia al cargo de evo morales quien fue acusado de fraude electoral el 13 de marzo áñez cumplió un año con detención preventiva acusada por el caso golpe de estado i al que posteriormente se sumó el caso golpe de estado ii actualment la asamblea legislativa tramita también un juicio de responsabilidades el ministro de justicia señaló que en el gobierno de añez no se implementó el trabajo del grupo interdisciplinario de expertos independientes gieibolivia áñez fue acusada por el ministerio público por los presuntos delitos de resoluciones contrarias a la constitución política del estado cpe e incumplimiento de deberes según lima un proceso penal no debería exceder los tres años / lmpt</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/25/coronavirus-seis-nuevos-casos-en-oruro-y-tres-pacientes-recuperados/</t>
+          <t>https://lapatria.bo/2022/03/27/lima-califica-como-historico-el-inicio-del-juicio-contra-anez/</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -788,51 +788,51 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>36a7cde7d7d990cff2e7a206f6095c19</t>
+          <t>bb5be82e9b2bf9b2789b3be318714164</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G7" t="n">
-        <v>1775</v>
+        <v>2291</v>
       </c>
       <c r="H7" t="n">
         <v>7</v>
       </c>
       <c r="I7" t="n">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>('oruro', 4)</t>
+          <t>('áñez', 6)</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>('machacamarca', 4)</t>
+          <t>('proceso', 6)</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>('carangas', 4)</t>
+          <t>('estado', 5)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>lima califica como histórico el inicio del juicio contra áñez</t>
+          <t>crecida del río piraí pone en riesgo al municipio de san pedro</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> el ministro de justicia y transparencia institucional iván lima calificó como “histórico” el inicio del juicio denominado golpe de estado ii contra la expresidente jeanine áñez y pidió a su defensa no interferir en el proceso con “chicanas políticas” “mañana es un día histórico esperamos que la defensa de jeanine áñez no obstaculice el debido proceso con ‘chicanas’ que solo afectan al debido proceso y el pedido de #memoriaverdadyjusticia” escribió lima en la cuenta de twitter del ministerio de justicia y transparencia institucional la exmandataria enfrentará un proceso por la vía ordinaria denominado golpe de estado ii que tiene previsto iniciar este jueves 28 en el tribunal 1º de sentencia anticorrupción de la paz el juicio debió iniciarse el 10 de febrero pero fue suspendido ante numerosas objeciones por parte de la acusada según informó el diario la razón pese a que la defensa de jeanine áñez advirtió que presentaría una serie de recursos para que este juicio sea presencial debido a su importancia según lo que argumentaron el proceso será virtual según el nuevo auto de apertura áñez fue acusada por asumir la presidencia del senado en noviembre de 2019 lo que posteriormente le permitió acceder al poder supuestamente sin cumplir el reglamento de debate ni los preceptos constitucionales la defensa legal de la exmandataria negó los cargos y argumentó que todos los procedimientos de sucesión estaban enmarcados en la norma la entonces senadora asumió la presidencia el 12 de noviembre de 2019 después de varios días de disturbios en el país que produjeron posteriormente la renuncia al cargo de evo morales quien fue acusado de fraude electoral el 13 de marzo áñez cumplió un año con detención preventiva acusada por el caso golpe de estado i al que posteriormente se sumó el caso golpe de estado ii actualment la asamblea legislativa tramita también un juicio de responsabilidades el ministro de justicia señaló que en el gobierno de añez no se implementó el trabajo del grupo interdisciplinario de expertos independientes gieibolivia áñez fue acusada por el ministerio público por los presuntos delitos de resoluciones contrarias a la constitución política del estado cpe e incumplimiento de deberes según lima un proceso penal no debería exceder los tres años / lmpt</t>
+          <t xml:space="preserve"> la crecida del río piraí originó un boquete cerca de los defensivos ubicados en el municipio de san pedro en el departamento de santa cruz el daño fue evaluado por la gobernación que desplazó una comisión hasta la zona afectada la comitiva llegó hasta la comunidad de hardemann y se adentró diez kilómetros en la zona de remanso donde se registró la crecida del río la madrugada del sábado ese incidente provocó el boquete o ruptura de los defensivos ejecutados anteriormente hasta el lugar se desplazaron la secretaría de desarrollo sostenible y medio ambiente del servicio de encauzamiento de aguas y regularización del río piraí searpi del servicio departamental de caminos sedcam y de la dirección de gestión de riesgos de acuerdo el deber según el equipo técnico de la gobernación cruceña este boquete puso en riesgo a las comunidades vecinas y áreas productivas como hardemann y litoral entre otras el responsable de cuencas del searpi josé antonio rivero aclaró que los trabajos en ese sector se realizan desde hace meses específicamente en la sección del río que no soporta el caudal del mismo rivero informó que la gobernación trabajó en la elaboración de un informe de la situación dado que mientras persista el turbión no se puede ejecutar ninguna acción una vez que se calme el movimiento de las aguas se tiene prevista una solución de emergencia o paliativa de acuerdo con el reporte técnico realizado se analizará el costo económico y las posibilidades de presupuesto del comité de operaciones de emergencia departamental coed mientras no se pueda trabajar en una solución el agua amenaza con llegar a comunidades ubicadas en lugares no aptos para el asentamiento legalmente el municipio de san pedro está clasificado como área de pradera lo que lo vuelve más propenso a inundaciones el secretario de desarrollo sostenible y medio ambiente jhonny rojas exhortó a las autoridades locales y nacionales a trabajar conjuntamente sin importar colores políticos esto para salvaguardar a los pobladores que están amenazados por la crecida del río / lmpt</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/27/lima-califica-como-historico-el-inicio-del-juicio-contra-anez/</t>
+          <t>https://lapatria.bo/2022/03/27/crecida-del-rio-pirai-pone-en-riesgo-al-municipio-de-san-pedro/</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -842,51 +842,51 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>bb5be82e9b2bf9b2789b3be318714164</t>
+          <t>ecb1632c47517007d9645114d2723b29</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G8" t="n">
-        <v>2291</v>
+        <v>2061</v>
       </c>
       <c r="H8" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I8" t="n">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>('áñez', 6)</t>
+          <t>('río', 5)</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>('proceso', 6)</t>
+          <t>('crecida', 3)</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>('estado', 5)</t>
+          <t>('boquete', 3)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>crecida del río piraí pone en riesgo al municipio de san pedro</t>
+          <t>reportan 2 nuevos casos de covid19 en oruro van 15 días sin fallecidos</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> la crecida del río piraí originó un boquete cerca de los defensivos ubicados en el municipio de san pedro en el departamento de santa cruz el daño fue evaluado por la gobernación que desplazó una comisión hasta la zona afectada la comitiva llegó hasta la comunidad de hardemann y se adentró diez kilómetros en la zona de remanso donde se registró la crecida del río la madrugada del sábado ese incidente provocó el boquete o ruptura de los defensivos ejecutados anteriormente hasta el lugar se desplazaron la secretaría de desarrollo sostenible y medio ambiente del servicio de encauzamiento de aguas y regularización del río piraí searpi del servicio departamental de caminos sedcam y de la dirección de gestión de riesgos de acuerdo el deber según el equipo técnico de la gobernación cruceña este boquete puso en riesgo a las comunidades vecinas y áreas productivas como hardemann y litoral entre otras el responsable de cuencas del searpi josé antonio rivero aclaró que los trabajos en ese sector se realizan desde hace meses específicamente en la sección del río que no soporta el caudal del mismo rivero informó que la gobernación trabajó en la elaboración de un informe de la situación dado que mientras persista el turbión no se puede ejecutar ninguna acción una vez que se calme el movimiento de las aguas se tiene prevista una solución de emergencia o paliativa de acuerdo con el reporte técnico realizado se analizará el costo económico y las posibilidades de presupuesto del comité de operaciones de emergencia departamental coed mientras no se pueda trabajar en una solución el agua amenaza con llegar a comunidades ubicadas en lugares no aptos para el asentamiento legalmente el municipio de san pedro está clasificado como área de pradera lo que lo vuelve más propenso a inundaciones el secretario de desarrollo sostenible y medio ambiente jhonny rojas exhortó a las autoridades locales y nacionales a trabajar conjuntamente sin importar colores políticos esto para salvaguardar a los pobladores que están amenazados por la crecida del río / lmpt</t>
+          <t xml:space="preserve"> el departamento de oruro cumplió este miércoles 15 días consecutivos sin reportar pacientes de coronavirus fallecidos mientras que los nuevos casos fueron dos hay una persona recuperada el reporte del servicio departamental de salud sedes detalla que los dos nuevos casos de coronavirus son del municipio de oruro en cambio la persona recuperada es de challapata en el informe diario de casos de coronavirus el sedes informó que no hubo variación en el total de contagios confirmados desde el inicio de la pandemia en oruro pero si se reasignaron algunos casos a diferentes municipios esto tras un control de calidad de la información que se recopila total hasta el momento en el departamento de oruro se registraron 42262 casos de coronavirus además 40584 pacientes se recuperaron 1594 fallecieron y hay 84 personas que todavía tienen el virus contagios con los nuevos contagios la ciudad capital suma 35537 casos seguida de huanuni con 1521 challapata 1143 machacamarca 392 caracollo 359 sabaya 288 turco 266 salinas de garci mendoza 238 antequera 218 eucaliptus 214 toledo 210 poopó 209 curahuara de carangas 196 huari 185 huachacalla 163 santiago de andamarca 154 pazña 149 corque 133 pampa aullagas 103 el choro 87 quillacas 83 en tanto totora 67 huayllamarca 66 soracachi 56 esmeralda 43 yunguyo de litoral 37 belén de andamarca 28 choquecota 26 cruz de machacamarca 26 escara 23 chipaya 21 coipasa 15 la rivera cinco carangas y todos santos uno recuperados el municipio de oruro acumula 34127 personas recuperadas huanuni 1469 challapata 1081 machacamarca 374 caracollo 335 sabaya 284 turco 264 salinas de garci mendoza 233 antequera 212 eucaliptus 202 toledo 201 poopó 194 curahuara de carangas 178 huari 177 huachacalla 157 santiago de andamarca 148 pazña 146 corque 131 pampa aullagas 101 el choro 87 quillacas 80 huayllamarca 65 finalmente totora 62 soracachi 55 esmeralda 42 yunguyo de litoral 36 belén de andamarca 28 choquecota 25 cruz de machacamarca 24 escara 23 chipaya 21 coipasa 15 la rivera cinco todos santos uno y carangas uno</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/27/crecida-del-rio-pirai-pone-en-riesgo-al-municipio-de-san-pedro/</t>
+          <t>https://lapatria.bo/2022/03/24/reportan-2-nuevos-casos-de-covid-19-en-oruro-van-15-dias-sin-fallecidos/</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -896,51 +896,51 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>ecb1632c47517007d9645114d2723b29</t>
+          <t>a9c33eb5a34006163637b2e83aaf4e96</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="G9" t="n">
-        <v>2061</v>
+        <v>2049</v>
       </c>
       <c r="H9" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I9" t="n">
-        <v>187</v>
+        <v>240</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>('río', 5)</t>
+          <t>('oruro', 5)</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>('crecida', 3)</t>
+          <t>('coronavirus', 4)</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>('boquete', 3)</t>
+          <t>('machacamarca', 4)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>uno de cada tres estudiantes ya tiene dos dosis de la vacuna anticovid</t>
+          <t>covid19 dos nuevos casos y dos recuperados este martes en oruro</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> después de un mes del retorno a clases presenciales en todo el país solo el 33 por ciento de los estudiantes recibieron el esquema completo de vacunas contra el coronavirus desde el gobierno instaron a los servicios departamentales de salud sedes a desplegar brigadas en las unidades educativas según datos del ministerio de salud hasta la fecha se inmunizaron con dos dosis a un millón de estudiantes entre cinco y 17 años este número representa el 33 por ciento de los tres millones de niños y adolescentes que viven en el país la semana precedente el ministro de sauld jeyson auza instó a los sedes a desplegar brigadas médicas en los colegios que estén pasando clases presenciales la autoridad aseguró que desde su despacho se desplegaron estos equipos en el área rural “esta actividad debe ser emulada copiada por los servicios departamentales de salud y todos los establecimientos que tienen en su área de intervención una unidad educativa” declaró auza la autoridad explicó que las tareas que se realizan desde su despacho para combatir el coronavirus son integrales porque no solo diagnostican y vacunan sino también brindan tratamientos y realizan trabajos de desparasitación según informó página seite desde la semana pasada el ministerio de salud y deportes desplegó a más de 2700 médicos en los centros educativos del área rural con el objetivo de preservar la salud de los estudiantes en esas zonas del país “instamos a las direcciones municipales y a los servicios departamentales de salud que tienen la fuerza operativa para realizar esta actividad que cumplan esta tarea instruida por el ministerio de salud” añadió el ministro por su parte el ministro de educación édgar pary chambi informó que las unidades educativas que presenten casos positivos de coronavirus deberán suspender temporalmente las labores presenciales y retomar las clases virtuales de cinco a site días en el “protocolo de bioseguridad para el retorno seguro a clases” elaborado por los ministerios de educación y salud se estipuló “la suspensión temporal de labores educativas en la modalidad de atención educativa presencial” cuando se confirma un caso positivo de covid el ministro de educación recalcó que las unidades educativas deben tomar inmediatamente las decisiones cuando se presentan contagios y no esperar determinaciones / lmpt</t>
+          <t xml:space="preserve"> los nuevos contagios de covid19 este martes en oruro fueron dos cifra similar se tuvo de pacientes recuperados además se cumplieron 14 días es decir dos semanas que no hay fallecidos con esta enfermedad en el departamento el reporte del servicio departamental de salud sedes precisa que las dos personas recuperadas son del municipio de oruro al igual que uno de los contagiados con el virus mientras que el restante nuevo caso es de challapata las bajas cifras se registraron a pesar de que se hicieron 339 pruebas el martes de las cuales 330 se descartaron porque dieron negativo dos fueron positivo dos sirvieron para dar alta médica y de las cinco restantes aún se aguarda su resultado   hasta el momento en el departamento de oruro se registraron 42260 casos de coronavirus además 40583 pacientes se recuperaron 1594 fallecieron y hay 83 personas que todavía tienen el virus con los nuevos contagios la ciudad capital suma 35525 casos seguida de huanuni con 1530 challapata 1143 machacamarca 392 caracollo 359 sabaya 288 turco 267 salinas de garci mendoza 238 antequera 218 eucaliptus 213 toledo 210 poopó 209 curahuara de carangas 196 huari 185 huachacalla 163 santiago de andamarca 154 pazña 149 corque 133 pampa aullagas 103 el choro 87 quillacas 83 en tanto totora 67 huayllamarca 66 soracachi 56 esmeralda 43 yunguyo de litoral 37 belén de andamarca 28 choquecota 26 cruz de machacamarca 25 escara 23 chipaya 21 coipasa 15 la rivera cinco carangas y todos santos uno el municipio de oruro acumula 34156 personas recuperadas huanuni 1466 challapata 1055 machacamarca 374 caracollo 335 sabaya 284 turco 264 salinas de garci mendoza 233 antequera 212 eucaliptus 201 toledo 201 poopó 194 curahuara de carangas 178 huari 177 huachacalla 157 santiago de andamarca 148 pazña 146 corque 131 pampa aullagas 101 el choro 87 quillacas 80 huayllamarca 65 finalmente totora 62 soracachi 55 esmeralda 42 yunguyo de litoral 36 belén de andamarca 28 choquecota 25 cruz de machacamarca 24 escara 23 chipaya 21 coipasa 15 la rivera cinco todos santos uno y carangas uno</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/27/uno-de-cada-tres-estudiantes-ya-tiene-dos-dosis-de-la-vacuna-anticovid/</t>
+          <t>https://lapatria.bo/2022/03/23/covid-19-dos-nuevos-casos-y-dos-recuperados-este-martes-en-oruro/</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -950,51 +950,51 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>b7fd5ec5158597067f9948d6f9785aac</t>
+          <t>375aedc5e999e438019a11c3ca4c8aea</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G10" t="n">
-        <v>2329</v>
+        <v>2062</v>
       </c>
       <c r="H10" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I10" t="n">
-        <v>216</v>
+        <v>248</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>('salud', 7)</t>
+          <t>('oruro', 4)</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>('desde', 4)</t>
+          <t>('machacamarca', 4)</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>('educativas', 4)</t>
+          <t>('carangas', 4)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>choquehuanca quiere nuevos líderes en el mas para que no se “desnaturalice”</t>
+          <t>cochabamba policía investiga muerte de una niña que llegó al hospital con signos de violencia</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> el vicepresidente del estado david choquehuanca exhortó la jornada precedente a dirigentes y militantes del movimiento al socialismo mas a apostar a la formación de nuevos líderes con el fin de que el partido mantenga su identidad propia y no se desnaturalice el pedido del vicepresidente ocurrió coincidentemente al mismo tiempo que las afirmaciones sobre la división dentro del movimiento al socialismo cobraron más fuerza especialmente en los últimos días dos ejemplos claros de esta situación fueron las expulsiones del partido del diputado rolando cuéllar y de la exdirigente de la confederación de mujeres interculturales de bolivia angélica ponce ambos por cuestionar la prolongada dirigencia de evo morales “tenemos que unirnos todos sino vamos a seguir detrás de una minoría no pueden seguir manejándonos los que dividen los que nos mienten los que nos roban los flojos estamos mal porque estamos divididos” manifestó choquehuanca ante una concentración en la población de coripata en los yungas de la paz el vicepresidente destacó la participación de los jóvenes y pidió apostar por las “wawas” quienes según choquehuanca son los que harán posible que el mas se levante con identidad propia según lo publicado por erbol “tenemos que apostar por nuevos líderes hay que apostar por nuestras wawas para levantarnos con identidad propia nuestro proceso es para recuperar nuestra identidad y dignidad tenemos que prepararnos para gobernarnos nosotros mismos” expresó la autoridad choquehuanca declaró estar dispuesto a ayudar en la formación de nuevos líderes con motivo de su visita a coripata se refirió específicamente a los jóvenes y señoritas yungueñas el vicepresidente incluso dedicó gran parte de su visita a dictar un curso en el recomendó estudiar filosofía economía política historia planificación gestión pública y sobre el estado plurinacional la autoridad también hizo alusión al 27 aniversario del movimiento al socialismo celebrado en horas precedentes y dijo que el deber de las personas que conforman esta fuerza política es trabajar para recuperar la esencia del partido “son 27 años que han pasado desde que creamos nuestro instrumento mismo que ahora corre el riesgo de desnaturalizarse necesitamos recuperar su esencia” manifestó choquehuanca / lmpt</t>
+          <t xml:space="preserve"> este viernes una madre y el padrastro llevaron el cuerpo sin vida de una niña de 1 año y 9 meses a un hospital de la zona sur de cochabamba ambos explicaron que la menor se había caído de una fuente la policía tras evidenciar que la niña tenía signos de violencia de larga data los arrestó a ambos con fines investigativos según información de los medios de comunicación la niña fue llevada al centro de salud de cerro verde cerca de las 0800 horas de hoy el servicio de emergencia realizó el examen correspondiente y no encontró signos vitales por lo que se realizó maniobras de resucitación sin resultados «al no encontrarse signos vitales se le realiza la resucitación cardiopulmonar por parte del médico de turno pero no fue factible porque no tuvimos una respuesta favorable se le diagnosticó un tec grave y sospecha de fractura de base de cráneo» informó la responsable del hospital la médico jaqueline mamani a red uno los médicos encontraron un hematoma a nivel de la cabeza en la región parietal además un ojo que estaba equimótico y edematizado había lesiones en el lado izquierdo y también un edema y equimosis hasta la región mandibular «el padre refiere que la menor se cayó de una altura de más o menos un metro él dijo que se cayó de la fuente y no se despertó al llegar la menor al hospital ya estaba sin signos vitales sin respuesta alguna» afirmó la responsable del hospital al tratarse de una menor de edad el servicio médico comunicó el hecho a la defensoría y a la felcc quienes llegaron al lugar y retiraron el cuerpo según red uno la fiscal departamental de cochabamba nuria gonzales informó que el ministerio público tomó conocimiento del caso y envió personal para los exámenes correspondientes «la menor en el examen físico registra lesiones de data antigua y una posible situación de agresión sexual por lo cual toda actividad investigativa se está desplegando» dijo gonzales el director de la fuerza especial de lucha contra el crimen felcc ronald tapia informó que el cuerpo de la niña presentaba lesiones de data antigua de hace siete u ocho días a nivel del rostro aparentemente por una caída «estamos a la espera de la autopsia el resultado nos ayudará a determinar lo que podría haber pasado con la menor momentáneamente y con fines investigativos tenemos a dos personas arrestadas que es la mamá y el padrastro posteriormente se determinará la situación legal de ambos» argumentó tapia /hnf/</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/27/choquehuanca-quiere-nuevos-lideres-en-el-mas-para-que-no-se-desnaturalice/</t>
+          <t>https://lapatria.bo/2022/03/25/cochabamba-policia-investiga-muerte-de-una-nina-que-llego-al-hospital-con-signos-de-violencia/</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1004,51 +1004,51 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>884349a478ba9086debe1fc65bf32b12</t>
+          <t>5cba75a780eb856f0ecd14d3aecead15</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="G11" t="n">
-        <v>2277</v>
+        <v>2426</v>
       </c>
       <c r="H11" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I11" t="n">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>('choquehuanca', 5)</t>
+          <t>('menor', 6)</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>('vicepresidente', 4)</t>
+          <t>('niña', 4)</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>('apostar', 4)</t>
+          <t>('hospital', 4)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>gualberti llama a practicar el perdón y la reconciliación en la familia</t>
+          <t>santa cruz falta de espacio para neonatos en terapia intensiva de maternidad es crítica hay bebés en sillones</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> el arzobispo de santa cruz monseñor sergio gualberti llamó la presente jornada a practicar el perdón y la reconciliación en las familias como señal de conversión y valentía con uno mismo además de ser una manera de reencontrarse con dios “el padre ama a sus hijos por el solo hecho que son sus hijos más allá de sus conductas” dijo gualberti en su homilía quien también relató la parábola del hijo pródigo la historia de un joven que luego de recibir la herencia de su padre abandonó el ceno familiar y despilfarró su dinero para finalmente regresar arrepentido a su hogar gualberti prosiguió su relato y dijo que el protagonista de esta historia tocó fondo hasta el punto de tener que compartir comida con los cerdos no perdió solo su dinero y a su familia sino también su libertad su identidad y su dignidad como persona el monseñor reflexionó a la feligresía e indicó que el primer paso para la conversión es entrar en uno mismo tener la valentía de sincerarse ante la conciencia propia y reconocer los pecados cometidos el segundo paso explicó gualberti es reconocer la necesidad que tiene cada uno del amor y la misericordia de dios seguida de la decisión de abandonar “cobijos malolientes en ruinas” y regresar a la casa paterna según lo publicado por erbol gualberti prosiguió su relato y narró que el padre del joven decidió acogerlo de nuevo sin expresar ningún reproche solo porque su regreso era suficiente para él se armó una fiesta por su retorno pidió que le traigan ropa sandalias y un anillo y le devolvió sus derechos de hijo el monseñor explicó que ese momento representa el verdadero encuentro con dios pero que no todos son capaces de entenderlo pues en el relato el hijo mayor se enoja con su padre al enterarse de la celebración armada para su hermano pese a sus errores cuando él no hizo más que obedecer de acuerdo con las palabras de guaberti el padre de ambos jóvenes buscó su reconciliación al decirle “hijo mío tú estás siempre conmigo y todo lo mío es tuyo” según el monseñor esos sentimientos de humildad misericordia y fraternidad son los que deben primar las relaciones de los humanos gualberti manifestó que al igual que en esta parábola el señor siempre está dispuesto a perdonar y es por eso que los corazones de las personas se llenan de esperanza “en nombre de cristo déjense reconciliar con dios” dijo en su mensaje al exhortar a los fieles a instaurar nuevas relaciones basadas en el amor la reconciliación el perdón la armonía y la paz / lmpt</t>
+          <t xml:space="preserve"> el servicio de terapia intensiva para neonatos de la maternidad percy boland en santa cruz está saturado el espacio es tan insuficiente que hasta tres recién nacidos deben compartir una servocuna el director del hospital mario herbas manifestó su preocupación por la situación que consideró como una emergencia pues pueden desatarse brotes de infecciones en los bebés lo que representaría una responsabilidad médicolegal para todo su equipo desde la gobernación de ese departamento informaron que 17 recién nacidos ya fueron trasladados a otros centros médicos de segundo nivel sin embargo esta medida es solo paliativa pues a criterio de herbas lo que se necesita es un nuevo hospital materno infantil reportó el diario el deber la jornada precedente el secretario de salud fernando pacheco solicitó al ministerio de salud la firma de un convenio que permita a los centros médicos privados dar atenciones del sistema único de salud sus especialmente a los bebés que requieren terapia intensiva los médicos que trabajan en la maternidad percy boland lamentaron que los recién nacidos deban compartir las servocunas pues no cuentan con el espacio ni los recursos necesarios para brindarles la atención que requieren un bebé que entra a terapia intensiva neonatal es prematuro requiere un tratamiento cuidadoso sin embargo debe compartir el espacio con al menos otros dos pacientes que un recién nacido comparta la cervocuna es potencialmente peligroso pues otra de las razones por las que los bebés requieren cuidados intensivos son las defensas bajas lo que los vuelve mucho más propensos a contraer cualquier infección los pacientes que salen de terapia intensiva y necesitan cuidados intermedios tampoco tienen un espacio al cual llegar es por eso que el hospital tubo que habilitar incluso sillones para atender a los recién nacidos que lo requieren debido a la precariedad y la falta de espacio en el centro de salud el personal médico debe redoblar sus esfuerzos para atender a los pacientes pues al tratarse de recién nacidos requieren de cuidados muy delicados como ayuda para respirar / lmpt</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/27/gualberti-llama-a-practicar-el-perdon-y-la-reconciliacion-en-la-familia/</t>
+          <t>https://lapatria.bo/2022/03/26/santa-cruz-falta-de-espacio-para-neonatos-en-terapia-intensiva-de-maternidad-es-critica-hay-bebes-en-sillones/</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1058,51 +1058,51 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>4d926a38d8dfa70d8a74fa6d988f74ce</t>
+          <t>3f1e863fb92161ecd3c6abe033120f02</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="G12" t="n">
-        <v>2483</v>
+        <v>2100</v>
       </c>
       <c r="H12" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="I12" t="n">
-        <v>238</v>
+        <v>194</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>('gualberti', 6)</t>
+          <t>('recién', 6)</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>('padre', 5)</t>
+          <t>('espacio', 5)</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>('monseñor', 4)</t>
+          <t>('nacidos', 5)</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ine denuncia desestabilización y politización del censo en santa cruz</t>
+          <t>bolivia registra 184 casos positivos de covid19</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> la denuncia de desestabilización y politización del censo de población y vivienda fue hecha por el director ejecutivo del instituto nacional de estadística ine humberto arandia quien también señaló como uno de los principales responsables al presidente de la asamblea legislativa cruceña zvonko matkovic “hay intereses que quieren politizar un proceso que es meramente técnico se quiso hacer ver que no invitamos a la gobernación cruceña a participar de la socialización totalmente falso en el caso de santa cruz participaron el rector de la universidad gabriel rené moreno vicente cuéllar y un exdirector del ine jorge akamine por lo que esta convocatoria fue abierta” afirmó arandia lamentó que haya un “doble discurso” por el rector de la casa superior de estudios cruceña pues en primera instancia ponderó las tareas previas al censo sin embargo dijo otra cosa después también reclamó por las declaraciones y acciones de zvonko matkovic “hace unas semanas el presidente de la asamblea legislativa departamental zvonko matkovic se hizo presente en las puertas del ine indicando que el director no lo quería recibir pero lo que nunca dijo después es que un día antes había recibido una carta por mi persona indicando que se le pedía otro día y el señor matkovic cumpliendo su función política declaró que el ine no lo quería recibir” declaró el director ejecutivo del ine indicó que el proceso del censo será explicado a la sociedad civil de los nueve departamentos del país y a las instituciones que así lo requieran según informó el portal de noticias innovapress arandia también se refirió a la elaboración de la boleta censal que actualmente está en su etapa preliminar y está siendo trabajada por expertos del país en colaboración con organizaciones internacionales “todos los trabajos que estamos realizando están siendo supervisados y analizados por una comisión internacional de alto nivel conformada por expertos internacionales en la temática censal el objetivo del censo tiene que ser avalado por técnicos de naciones unidas la cepal/celade banco mundial banco interamericano de desarrollo y fonplata” explicó en cuanto al presupuesto para el censo arandia explicó que el ine cuenta con 181 millones bolivianos de los cuales 65 fueron otorgados a través del decreto supremo 4664 y serán destinados a la contratación de consultores para llevar adelante el proceso censal además de otros 116 millones de bolivianos entregados mediante trasferencia presupuestaria por el ministerio de economía y finanzas públicas / lmpt</t>
+          <t xml:space="preserve"> la desescalada de casos persiste en el país al igual que el incremento de pacientes recuperados con 1963 registrados la presente jornada además de no reportarse decesos por el virus en bolivia se registraron 184 casos positivos de coronavirus este sábado según los datos del ministerio de salud y deportes santa cruz 33 cochabamba 18 la paz 107 chuquisaca cinco tarija uno potosí 18 oruro dos beni ninguno y pando ninguno total el país registra hasta el momento un total de 901292 casos positivos de coronavirus de los cuales 829710 son pacientes recuperados el número de decesos asciende a 21487 y actualmente hay 50095 casos activos vacunados el reporte de vacunación diario del ministerio de salud detalla que hasta la fecha 6074507 personas recibieron la primera dosis de éstas 4784783 tienen la segunda y 1208408 la tercera además 994961 ciudadanos cuentan con la vacuna janssen de una sola dosis desde la cartera de salud y deportes anuncian que hasta el sábado se aplicaron 13062659 dosis de las vacunas sputnikv astrazeneca sinopharm pfizer y janssen en todo el territorio nacional</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/27/ine-denuncia-desestabilizacion-y-politizacion-del-censo-en-santa-cruz/</t>
+          <t>https://lapatria.bo/2022/03/26/bolivia-registra-184-casos-positivos-de-covid-19/</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1112,34 +1112,34 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>513d38dbc59bb31bc88e3af03a1815e4</t>
+          <t>0577f82b653a440188bea2ca0351b10d</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="G13" t="n">
-        <v>2531</v>
+        <v>1090</v>
       </c>
       <c r="H13" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I13" t="n">
-        <v>235</v>
+        <v>109</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>('ine', 6)</t>
+          <t>('salud', 3)</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>('censo', 5)</t>
+          <t>('hasta', 3)</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>('arandia', 4)</t>
+          <t>('dosis', 3)</t>
         </is>
       </c>
     </row>
@@ -1200,17 +1200,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>covid19 oruro no reporta casos nuevos esta jornada</t>
+          <t>la paz envían a la cárcel a militar acusado de ayudar a escapar a su hijo presunto feminicida de vania</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> la jornada del 27 de marzo oruro no registró nuevos casos de coronavirus de igual manera se mantuvieron los cero decesos con lo que se cumplieron 19 días con la misma tendencia el reporte del servicio departamental de salud sedes indicó la recuperación de dos pacientes ambos del municipio de oruro y se descartaron 150 casos en esta jornada total con este reporte el municipio de oruro se mantiene con un total de 35549 casos positivos de coronavirus y 34138 pacientes recuperados actualmente hay 87 casos activos contagios debido a la ausencia de contagios en esta jornada la capital se mantiene con 35549 casos positivos de coronavirus seguida huanuni con 1512 casos callapata 1143 machacamarca 392 caracollo 359 sabaya 288 turco 266 salinas de garci mendoza 238 antequera 218 y eucaliptos con 214 casos curahuara de carangas se mantiene con 196 casos al igual que huari con 185 positivos huachacalla 163 santiago de andamarca 154 pazña 149 corque 133 pampa aullagas 103 el choro 87 quillacas 83 en tanto totora 67 huayllamarca 66 soracachi 56 esmeralda 43 yunguyo de litoral 37 belén de andamarca 28 choquecota 26 cruz de machacamarca 26 escara 23 chipaya 21 coipasa 15 la rivera cinco carangas y todos santos uno recuperados ya son 34138 pacientes recuperados en el municipio de oruro huanuni 1469 challapata 1081 machacamarca 374 caracollo 335 sabaya 284 turco 264 salinas de garci mendoza 233 antequera 212 eucaliptus 202 toledo 201 poopó 194 curahuara de carangas se mantiene con 178 pacientes recuperados huari 177 huachacalla 157 santiago de andamarca 148 pazña 146 corque 131 pampa aullagas 101 el choro 87 quillacas 80 huayllamarca 65 finalmente totora 62 soracachi 55 esmeralda 42 yunguyo de litoral 36 belén de andamarca 28 choquecota 25 cruz de machacamarca 24 escara 23 chipaya 21 coipasa 15 la rivera cinco todos santos uno y finalmente carangas uno</t>
+          <t xml:space="preserve"> el teniente coronel del ejército iván li padre del presunto feminicida de vania t b fue enviado a la cárcel de san pedro de la ciudad de la paz con detención preventiva mientras duran las investigaciones del caso el plazo de la detención preventiva es de cinco meses mientras se realiza la investigación informó el coronel jhonny vega director de la fuerza especial de lucha contra la violencia felcv “el militar está acusado de autoría mediata en el caso puesto que habría ayudado a la fuga de su hijo” indicó el coronel vega el caso de feminicidio de vania fue registrado el 18 de febrero según la investigación el presunto autor vladimir iv hijo del militar detenido habría dicho que la víctima falleció por ingerir una sustancia tóxica pero se evidenció que fue estrangulada el pasado viernes el militar fue aprehendido y se realizó un allanamiento en su domicilio en la cual se secuestraron dos celulares informó el coronel vega la policía continúa en la búsqueda del prófugo vladimir iv /hnf/</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/27/covid-19-oruro-no-reporta-casos-nuevos-esta-jornada/</t>
+          <t>https://lapatria.bo/2022/03/21/la-paz-envian-a-la-carcel-a-militar-acusado-de-ayudar-a-escapar-a-su-hijo-presunto-feminicida-de-vania/</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1220,51 +1220,51 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>87e105763ba8a5acb2040ebdefe841e4</t>
+          <t>101ab6d3a2944285f73df6c296524788</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="G15" t="n">
-        <v>1867</v>
+        <v>999</v>
       </c>
       <c r="H15" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="I15" t="n">
-        <v>224</v>
+        <v>99</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>('oruro', 4)</t>
+          <t>('coronel', 4)</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>('pacientes', 4)</t>
+          <t>('caso', 3)</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>('mantiene', 4)</t>
+          <t>('vega', 3)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>moisés villarroel el nuevo capitán de la selección boliviana “tenemos que trabajar todavía mucho”</t>
+          <t>uno de cada tres estudiantes ya tiene dos dosis de la vacuna anticovid</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> “tenemos que trabajar todavía mucho más cada uno en su club y cuando vengamos a la selección hacer lo mejor posible y darle una alegría al país” declaró moisés villarroel mediocampista y capitán del seleccionado verde después de la derrota ante colombia 03 en la ciudad de barranquilla el elenco renovado convocado para la recta final de las eliminatorias a la copa mundial catar 2022 aguantó la presión de colombia desde el inicio de las acciones y soportó 39 minutos con el marcador en blanco después de este esfuerzo el cuadro amarillo pasó adelante en el marcador hasta quedarse con los tres puntos y revivir su ilusión de llegar al mundial “se nos complicó con el 10 estamos haciendo antes del primer gol un partido bueno tácticamente estábamos muy ordenados y sólo nos queda trabajar” indicó villarroel quien a sus 23 años por primera vez llevó el cintillo de capitán de la selección absoluta los errores defensivos en la marcación ante los centros y la falta de ajuste en la marcación dejaron a bolivia descubierta y a colombia como el dominador del compromiso el cuadro verde jugó agazapado en su área sin insinuar ninguna ocasión de verdadero peligro villarroel admitió las fallas del equipo “si hacíamos mejor lo que teníamos que hacer íbamos a tratar de llevarnos aunque sea el empate” el volante fue reemplazado a los 84 minutos por gabriel villamil cuando el marcador estaba 20 el director técnico césar farías mandó al terreno un plantel renovado al ver que bolivia tenía recudidas las chances de pelear por ingresar a la zona de repechaje y esta primera experiencia en conjunto fue calificada como alentadora por villarroel “como vieron en la cancha había bastantes jóvenes 22 y 23 años y es una nueva camada son jugadores que quiere que bolivia salga adelante que bolivia mejore pero es con mucho trabajo” declaró villarroel quien volverá a ser titular en el equipo que farías preparará para la despedida de estas eliminatorias el siguiente partido de bolivia será contra brasil el martes 29 de marzo a partir de las 1930 en el estadio “hernando siles” de la paz donde tratará de cerrar su actuación con una victoria</t>
+          <t xml:space="preserve"> después de un mes del retorno a clases presenciales en todo el país solo el 33 por ciento de los estudiantes recibieron el esquema completo de vacunas contra el coronavirus desde el gobierno instaron a los servicios departamentales de salud sedes a desplegar brigadas en las unidades educativas según datos del ministerio de salud hasta la fecha se inmunizaron con dos dosis a un millón de estudiantes entre cinco y 17 años este número representa el 33 por ciento de los tres millones de niños y adolescentes que viven en el país la semana precedente el ministro de sauld jeyson auza instó a los sedes a desplegar brigadas médicas en los colegios que estén pasando clases presenciales la autoridad aseguró que desde su despacho se desplegaron estos equipos en el área rural “esta actividad debe ser emulada copiada por los servicios departamentales de salud y todos los establecimientos que tienen en su área de intervención una unidad educativa” declaró auza la autoridad explicó que las tareas que se realizan desde su despacho para combatir el coronavirus son integrales porque no solo diagnostican y vacunan sino también brindan tratamientos y realizan trabajos de desparasitación según informó página seite desde la semana pasada el ministerio de salud y deportes desplegó a más de 2700 médicos en los centros educativos del área rural con el objetivo de preservar la salud de los estudiantes en esas zonas del país “instamos a las direcciones municipales y a los servicios departamentales de salud que tienen la fuerza operativa para realizar esta actividad que cumplan esta tarea instruida por el ministerio de salud” añadió el ministro por su parte el ministro de educación édgar pary chambi informó que las unidades educativas que presenten casos positivos de coronavirus deberán suspender temporalmente las labores presenciales y retomar las clases virtuales de cinco a site días en el “protocolo de bioseguridad para el retorno seguro a clases” elaborado por los ministerios de educación y salud se estipuló “la suspensión temporal de labores educativas en la modalidad de atención educativa presencial” cuando se confirma un caso positivo de covid el ministro de educación recalcó que las unidades educativas deben tomar inmediatamente las decisiones cuando se presentan contagios y no esperar determinaciones / lmpt</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/25/moises-villarroel-el-nuevo-capitan-de-la-seleccion-boliviana-tenemos-que-trabajar-todavia-mucho/</t>
+          <t>https://lapatria.bo/2022/03/27/uno-de-cada-tres-estudiantes-ya-tiene-dos-dosis-de-la-vacuna-anticovid/</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1274,51 +1274,51 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>69389eb8af8c6620eab8c809dfa1eca0</t>
+          <t>b7fd5ec5158597067f9948d6f9785aac</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="G16" t="n">
-        <v>2133</v>
+        <v>2329</v>
       </c>
       <c r="H16" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I16" t="n">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>('villarroel', 5)</t>
+          <t>('salud', 7)</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>('bolivia', 5)</t>
+          <t>('desde', 4)</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>('colombia', 3)</t>
+          <t>('educativas', 4)</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>cuatro regiones del país están aisladas por bloqueos</t>
+          <t>gualberti llama a practicar el perdón y la reconciliación en la familia</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> se cumplió una semana desde que se iniciaron los bloqueos en el desaguadero buena vista y en ascensión de guarayos que mantienen aislado parte del eje central del país el gobierno no logra concretar las soluciones necesarias para la resolución de los conflictos y el levantamiento de las medidas de presión la confederación de empresarios privados de bolivia cepb pidió priorizar el diálogo para que se levanten los bloqueos en distintos puntos del país ya que estas medidas de presión solo generan pérdidas económicas cuantiosas “los conflictos sociales que resultan en cierre de carreteras generan pérdidas cuantiosas al transporte comercio e industria y golpean aún más a las empresas ya afectadas por la pandemia y la crisis mundial urge diálogo” fue la petición de los empresarios privados el bloqueo en ascensión de guarayos impide el paso entre santa cruz y beni el de buena vista cerró el flujo vehicular entre santa cruz cochabamba y la paz en el desaguadero el movimiento comercial por la carretera a perú se vio afectado por las medidas de presión en ascensión de guarayos en la comunidad san antonio de la junta el conflicto se debe a que unos comunarios exigen la titulación de un predio incautado hace dos semanas la semana precedente incluso se registraron enfrentamientos entre estas personas y otro grupo que trató de desaojarlos según informó el deber los enfrentamientos dejaron el saldo de una persona fallecida identificada como franklin delgadillo después de este incidente los considerados avasalladores también instalaron un punto de bloqueo exigiendo el arresto de los responsables de esta muerte y que el terreno en cuestión sea adjudicado a su nombre en buena vista son las juntas escolares las que decidieron bloquear la carretera santa cruz cochabamba demandando un bono escolar que fue prometido por el alcalde del lugar pero que no se concretó hasta el momento los intentos de diálogo con ese sector fracasaron y la tensión entre bloqueadores y transportistas afectados creció en la paz comunidades de la provincia de ingavi cumplieron su séptimo día de bloqueos quienes entraron en conflicto por la construcción de la carretera doble vía río secodesaguadero la negativa de la gobernación paceña a pagar el 20 por ciento para la contraparte del proyecto carretero agravó la situación / lmpt</t>
+          <t xml:space="preserve"> el arzobispo de santa cruz monseñor sergio gualberti llamó la presente jornada a practicar el perdón y la reconciliación en las familias como señal de conversión y valentía con uno mismo además de ser una manera de reencontrarse con dios “el padre ama a sus hijos por el solo hecho que son sus hijos más allá de sus conductas” dijo gualberti en su homilía quien también relató la parábola del hijo pródigo la historia de un joven que luego de recibir la herencia de su padre abandonó el ceno familiar y despilfarró su dinero para finalmente regresar arrepentido a su hogar gualberti prosiguió su relato y dijo que el protagonista de esta historia tocó fondo hasta el punto de tener que compartir comida con los cerdos no perdió solo su dinero y a su familia sino también su libertad su identidad y su dignidad como persona el monseñor reflexionó a la feligresía e indicó que el primer paso para la conversión es entrar en uno mismo tener la valentía de sincerarse ante la conciencia propia y reconocer los pecados cometidos el segundo paso explicó gualberti es reconocer la necesidad que tiene cada uno del amor y la misericordia de dios seguida de la decisión de abandonar “cobijos malolientes en ruinas” y regresar a la casa paterna según lo publicado por erbol gualberti prosiguió su relato y narró que el padre del joven decidió acogerlo de nuevo sin expresar ningún reproche solo porque su regreso era suficiente para él se armó una fiesta por su retorno pidió que le traigan ropa sandalias y un anillo y le devolvió sus derechos de hijo el monseñor explicó que ese momento representa el verdadero encuentro con dios pero que no todos son capaces de entenderlo pues en el relato el hijo mayor se enoja con su padre al enterarse de la celebración armada para su hermano pese a sus errores cuando él no hizo más que obedecer de acuerdo con las palabras de guaberti el padre de ambos jóvenes buscó su reconciliación al decirle “hijo mío tú estás siempre conmigo y todo lo mío es tuyo” según el monseñor esos sentimientos de humildad misericordia y fraternidad son los que deben primar las relaciones de los humanos gualberti manifestó que al igual que en esta parábola el señor siempre está dispuesto a perdonar y es por eso que los corazones de las personas se llenan de esperanza “en nombre de cristo déjense reconciliar con dios” dijo en su mensaje al exhortar a los fieles a instaurar nuevas relaciones basadas en el amor la reconciliación el perdón la armonía y la paz / lmpt</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/25/cuatro-regiones-del-pais-estan-aisladas-por-bloqueos/</t>
+          <t>https://lapatria.bo/2022/03/27/gualberti-llama-a-practicar-el-perdon-y-la-reconciliacion-en-la-familia/</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1328,51 +1328,51 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>e25fd051c1a807a7590167ea247c5ea7</t>
+          <t>4d926a38d8dfa70d8a74fa6d988f74ce</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="G17" t="n">
-        <v>2322</v>
+        <v>2483</v>
       </c>
       <c r="H17" t="n">
         <v>6</v>
       </c>
       <c r="I17" t="n">
-        <v>209</v>
+        <v>235</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>('bloqueos', 3)</t>
+          <t>('gualberti', 6)</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>('buena', 3)</t>
+          <t>('padre', 5)</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>('vista', 3)</t>
+          <t>('monseñor', 4)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>reportan 2 nuevos casos de covid19 en oruro van 15 días sin fallecidos</t>
+          <t>choquehuanca quiere nuevos líderes en el mas para que no se “desnaturalice”</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> el departamento de oruro cumplió este miércoles 15 días consecutivos sin reportar pacientes de coronavirus fallecidos mientras que los nuevos casos fueron dos hay una persona recuperada el reporte del servicio departamental de salud sedes detalla que los dos nuevos casos de coronavirus son del municipio de oruro en cambio la persona recuperada es de challapata en el informe diario de casos de coronavirus el sedes informó que no hubo variación en el total de contagios confirmados desde el inicio de la pandemia en oruro pero si se reasignaron algunos casos a diferentes municipios esto tras un control de calidad de la información que se recopila total hasta el momento en el departamento de oruro se registraron 42262 casos de coronavirus además 40584 pacientes se recuperaron 1594 fallecieron y hay 84 personas que todavía tienen el virus contagios con los nuevos contagios la ciudad capital suma 35537 casos seguida de huanuni con 1521 challapata 1143 machacamarca 392 caracollo 359 sabaya 288 turco 266 salinas de garci mendoza 238 antequera 218 eucaliptus 214 toledo 210 poopó 209 curahuara de carangas 196 huari 185 huachacalla 163 santiago de andamarca 154 pazña 149 corque 133 pampa aullagas 103 el choro 87 quillacas 83 en tanto totora 67 huayllamarca 66 soracachi 56 esmeralda 43 yunguyo de litoral 37 belén de andamarca 28 choquecota 26 cruz de machacamarca 26 escara 23 chipaya 21 coipasa 15 la rivera cinco carangas y todos santos uno recuperados el municipio de oruro acumula 34127 personas recuperadas huanuni 1469 challapata 1081 machacamarca 374 caracollo 335 sabaya 284 turco 264 salinas de garci mendoza 233 antequera 212 eucaliptus 202 toledo 201 poopó 194 curahuara de carangas 178 huari 177 huachacalla 157 santiago de andamarca 148 pazña 146 corque 131 pampa aullagas 101 el choro 87 quillacas 80 huayllamarca 65 finalmente totora 62 soracachi 55 esmeralda 42 yunguyo de litoral 36 belén de andamarca 28 choquecota 25 cruz de machacamarca 24 escara 23 chipaya 21 coipasa 15 la rivera cinco todos santos uno y carangas uno</t>
+          <t xml:space="preserve"> el vicepresidente del estado david choquehuanca exhortó la jornada precedente a dirigentes y militantes del movimiento al socialismo mas a apostar a la formación de nuevos líderes con el fin de que el partido mantenga su identidad propia y no se desnaturalice el pedido del vicepresidente ocurrió coincidentemente al mismo tiempo que las afirmaciones sobre la división dentro del movimiento al socialismo cobraron más fuerza especialmente en los últimos días dos ejemplos claros de esta situación fueron las expulsiones del partido del diputado rolando cuéllar y de la exdirigente de la confederación de mujeres interculturales de bolivia angélica ponce ambos por cuestionar la prolongada dirigencia de evo morales “tenemos que unirnos todos sino vamos a seguir detrás de una minoría no pueden seguir manejándonos los que dividen los que nos mienten los que nos roban los flojos estamos mal porque estamos divididos” manifestó choquehuanca ante una concentración en la población de coripata en los yungas de la paz el vicepresidente destacó la participación de los jóvenes y pidió apostar por las “wawas” quienes según choquehuanca son los que harán posible que el mas se levante con identidad propia según lo publicado por erbol “tenemos que apostar por nuevos líderes hay que apostar por nuestras wawas para levantarnos con identidad propia nuestro proceso es para recuperar nuestra identidad y dignidad tenemos que prepararnos para gobernarnos nosotros mismos” expresó la autoridad choquehuanca declaró estar dispuesto a ayudar en la formación de nuevos líderes con motivo de su visita a coripata se refirió específicamente a los jóvenes y señoritas yungueñas el vicepresidente incluso dedicó gran parte de su visita a dictar un curso en el recomendó estudiar filosofía economía política historia planificación gestión pública y sobre el estado plurinacional la autoridad también hizo alusión al 27 aniversario del movimiento al socialismo celebrado en horas precedentes y dijo que el deber de las personas que conforman esta fuerza política es trabajar para recuperar la esencia del partido “son 27 años que han pasado desde que creamos nuestro instrumento mismo que ahora corre el riesgo de desnaturalizarse necesitamos recuperar su esencia” manifestó choquehuanca / lmpt</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/24/reportan-2-nuevos-casos-de-covid-19-en-oruro-van-15-dias-sin-fallecidos/</t>
+          <t>https://lapatria.bo/2022/03/27/choquehuanca-quiere-nuevos-lideres-en-el-mas-para-que-no-se-desnaturalice/</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1382,51 +1382,51 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>a9c33eb5a34006163637b2e83aaf4e96</t>
+          <t>884349a478ba9086debe1fc65bf32b12</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="G18" t="n">
-        <v>2049</v>
+        <v>2277</v>
       </c>
       <c r="H18" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I18" t="n">
-        <v>245</v>
+        <v>206</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>('oruro', 5)</t>
+          <t>('choquehuanca', 5)</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>('coronavirus', 4)</t>
+          <t>('vicepresidente', 4)</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>('machacamarca', 4)</t>
+          <t>('apostar', 4)</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>covid19 dos nuevos casos y dos recuperados este martes en oruro</t>
+          <t>covid19 oruro no reporta casos nuevos esta jornada</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> los nuevos contagios de covid19 este martes en oruro fueron dos cifra similar se tuvo de pacientes recuperados además se cumplieron 14 días es decir dos semanas que no hay fallecidos con esta enfermedad en el departamento el reporte del servicio departamental de salud sedes precisa que las dos personas recuperadas son del municipio de oruro al igual que uno de los contagiados con el virus mientras que el restante nuevo caso es de challapata las bajas cifras se registraron a pesar de que se hicieron 339 pruebas el martes de las cuales 330 se descartaron porque dieron negativo dos fueron positivo dos sirvieron para dar alta médica y de las cinco restantes aún se aguarda su resultado   hasta el momento en el departamento de oruro se registraron 42260 casos de coronavirus además 40583 pacientes se recuperaron 1594 fallecieron y hay 83 personas que todavía tienen el virus con los nuevos contagios la ciudad capital suma 35525 casos seguida de huanuni con 1530 challapata 1143 machacamarca 392 caracollo 359 sabaya 288 turco 267 salinas de garci mendoza 238 antequera 218 eucaliptus 213 toledo 210 poopó 209 curahuara de carangas 196 huari 185 huachacalla 163 santiago de andamarca 154 pazña 149 corque 133 pampa aullagas 103 el choro 87 quillacas 83 en tanto totora 67 huayllamarca 66 soracachi 56 esmeralda 43 yunguyo de litoral 37 belén de andamarca 28 choquecota 26 cruz de machacamarca 25 escara 23 chipaya 21 coipasa 15 la rivera cinco carangas y todos santos uno el municipio de oruro acumula 34156 personas recuperadas huanuni 1466 challapata 1055 machacamarca 374 caracollo 335 sabaya 284 turco 264 salinas de garci mendoza 233 antequera 212 eucaliptus 201 toledo 201 poopó 194 curahuara de carangas 178 huari 177 huachacalla 157 santiago de andamarca 148 pazña 146 corque 131 pampa aullagas 101 el choro 87 quillacas 80 huayllamarca 65 finalmente totora 62 soracachi 55 esmeralda 42 yunguyo de litoral 36 belén de andamarca 28 choquecota 25 cruz de machacamarca 24 escara 23 chipaya 21 coipasa 15 la rivera cinco todos santos uno y carangas uno</t>
+          <t xml:space="preserve"> la jornada del 27 de marzo oruro no registró nuevos casos de coronavirus de igual manera se mantuvieron los cero decesos con lo que se cumplieron 19 días con la misma tendencia el reporte del servicio departamental de salud sedes indicó la recuperación de dos pacientes ambos del municipio de oruro y se descartaron 150 casos en esta jornada total con este reporte el municipio de oruro se mantiene con un total de 35549 casos positivos de coronavirus y 34138 pacientes recuperados actualmente hay 87 casos activos contagios debido a la ausencia de contagios en esta jornada la capital se mantiene con 35549 casos positivos de coronavirus seguida huanuni con 1512 casos callapata 1143 machacamarca 392 caracollo 359 sabaya 288 turco 266 salinas de garci mendoza 238 antequera 218 y eucaliptos con 214 casos curahuara de carangas se mantiene con 196 casos al igual que huari con 185 positivos huachacalla 163 santiago de andamarca 154 pazña 149 corque 133 pampa aullagas 103 el choro 87 quillacas 83 en tanto totora 67 huayllamarca 66 soracachi 56 esmeralda 43 yunguyo de litoral 37 belén de andamarca 28 choquecota 26 cruz de machacamarca 26 escara 23 chipaya 21 coipasa 15 la rivera cinco carangas y todos santos uno recuperados ya son 34138 pacientes recuperados en el municipio de oruro huanuni 1469 challapata 1081 machacamarca 374 caracollo 335 sabaya 284 turco 264 salinas de garci mendoza 233 antequera 212 eucaliptus 202 toledo 201 poopó 194 curahuara de carangas se mantiene con 178 pacientes recuperados huari 177 huachacalla 157 santiago de andamarca 148 pazña 146 corque 131 pampa aullagas 101 el choro 87 quillacas 80 huayllamarca 65 finalmente totora 62 soracachi 55 esmeralda 42 yunguyo de litoral 36 belén de andamarca 28 choquecota 25 cruz de machacamarca 24 escara 23 chipaya 21 coipasa 15 la rivera cinco todos santos uno y finalmente carangas uno</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/23/covid-19-dos-nuevos-casos-y-dos-recuperados-este-martes-en-oruro/</t>
+          <t>https://lapatria.bo/2022/03/27/covid-19-oruro-no-reporta-casos-nuevos-esta-jornada/</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1436,51 +1436,51 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>375aedc5e999e438019a11c3ca4c8aea</t>
+          <t>87e105763ba8a5acb2040ebdefe841e4</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="G19" t="n">
-        <v>2062</v>
+        <v>1867</v>
       </c>
       <c r="H19" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I19" t="n">
-        <v>257</v>
+        <v>220</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>('dos', 5)</t>
+          <t>('oruro', 4)</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>('oruro', 4)</t>
+          <t>('pacientes', 4)</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>('uno', 4)</t>
+          <t>('mantiene', 4)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>rusia da por concluida la “primera fase” de la invasión a ucrania</t>
+          <t>exfuncionario de la cns fue aprehendido por la policía acusado de estafar ofreciendo cargos</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> rusia dio por concluida la “primera fase” de la invasión a ucrania que comenzó el 24 de febrero el anuncio se tradujo como el reconocimiento de que los objetivos planteados cuando iniciaron las operaciones militares no fueron alcanzados el jefe del principal departamento operativo del estado mayor de las fuerzas armadas de rusia sergey rudskoy dijo la jornada precedente que a un mes de que iniciaron las operaciones militares ahora los esfuerzos se centrarán en conseguir la “liberación total” de la región del donbás al este de ucrania el jefe militar también explicó que se consideraron dos opciones para su “operación especial militar” la primera consistía en abarcar toda ucrania y la segunda se enfocaba solo en el donbás según informó el portal de la bbc rudskoy aseguró que el 93% de luhansk y el 54% de donetsk ambas en la región de donbás están bajo control de las tropas rusas estos dos lugares fueron reconocidos por el presidente ruso vladimir putin como repúblicas independientes las declaraciones de rudskoy publicadas por las agencias de noticias estatales rusas apuntan a una posible reducción de los objetivos de guerra de rusia esto después de que las tropas de ese país encontraran una fuerte resistencia al norte de ucrania y especialmente en kiev la capital lo que marcó un “final exitoso” de la primera fase de las operaciones militares según rudskoy fue la destrucción de gran parte de la fuerza aérea y la armada ucraniana el ministerio de defensa ruso no descartó realizar operaciones militares en las ciudades que fueron bloqueadas además afirmaron que rusia reaccionará inmediatamente ante cualquier movimiento para cerrar el espacio aéreo sobre territorio ucraniano algo que el presidente de ese país volodymyr zelensky sigue pidiendo insistentemente la jornada precedente por segunda vez desde el inicio de la invasión el ministerio de defensa ruso dio un informe sobre las bajas en sus tropas reportaron 1351 soldados muertos y 3825 heridos sin embargo fuentes militares ucranianas afirmaron que al menos 15 mil soldados rusos murieron desde el inicio del conflicto aunque esta cifra podría incluir también heridos la inteligencia estadounidense sugiere una cifra más precisa puede ser solo la mitad de ese número / lmpt</t>
+          <t xml:space="preserve"> un hombre identificado como mauricio p r fue aprehendido por efectivos de la policía boliviana quien es acusado de presuntamente estafar a varias personas ofreciéndoles cargos en la caja nacional de salud cns a cambio de dinero informó el ministro de gobierno eduardo del castillo a los medios de comunicación “el señor oscar u m la señora mayra r c el señor isael g r y el señor josé luis c g habrían denunciado que existiría un exfuncionario de la caja nacional de salud que estaba cobrando distintas cantidades de dinero para incorporarlos y que presten servicios al interior de la caja nacional de salud la policía boliviana realizó el operativo correspondiente logrando la aprehensión de este exfuncionario” informó del castillo el ministro presentó este lunes a mauricio p r quien es exfuncionario de la unidad de recursos humanos de la cns y presuntamente cobraba distintas cantidades de dinero para incorporar a las víctimas a dicha institución durante el operativo policial se secuestraron distintas cantidades de dinero entre dólares y bolivianos además de dos equipos de telefonía móvil y documentación que servirá para el proceso de investigación este ciudadano cobraba entre bs 5000 y 22000 a sus víctimas “le pedimos a todo el pueblo boliviano que acuda a las instancias correspondientes para ver si tenemos sujetos como estos que se quieren aprovechar de la buena fe de las y los ciudadanos bolivianos” aseveró del castillo /hnf/</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/26/rusia-da-por-concluida-la-primera-fase-de-la-invasion-a-ucrania/</t>
+          <t>https://lapatria.bo/2022/03/21/exfuncionario-de-la-cns-fue-aprehendido-por-la-policia-acusado-de-estafar-ofreciendo-cargos/</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1490,51 +1490,51 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>bae380998c4b801c18fd320bf4a43cd0</t>
+          <t>ceeb8df104b6ed583966bfc82015fc8c</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="G20" t="n">
-        <v>2254</v>
+        <v>1445</v>
       </c>
       <c r="H20" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I20" t="n">
-        <v>211</v>
+        <v>140</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>('militares', 5)</t>
+          <t>('r', 4)</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>('rusia', 4)</t>
+          <t>('dinero', 4)</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>('ucrania', 4)</t>
+          <t>('caja', 3)</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>dan cuarto intermedio al bloqueo en la ruta a desaguadero</t>
+          <t>bolivia registra 75 nuevos casos de covid19</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dirigentes de la provincia ingavi anunciaron un cuarto intermedio de 15 días en los bloqueos en la ruta a desaguadero pese a que no se llegó a un acuerdo entre el gobierno y la gobernación de la paz la medida de presión ocasionó que cientos de camiones de carga internacional tanto de bolivia como de perú se vean perjudicados en el comercio de exportación e importación reportó la red erbol  la secretaria ejecutiva de la provincia ingavi maría eugenia millares hizo el anuncio en declaraciones a los medios durante una vigilia en el centro de la ciudad de la paz «se levanta el bloqueo damos un cuarto intermedio de 15 días» manifestóaceptan postura del gobierno y de la gobernación paceña amismo resaltó que los comunarios de la provincia ingavi aceptaron el compromiso de financiamiento del 80% por parte del gobierno y del 10% por parte de la gobernación de la paz para la construcción de la doble vía rio seco – desaguadero respecto al 10% restante indicó que evaluarán la forma de buscar de algún lado el financiamiento“nos sentimos ganadores porque no teníamos ni un 5% garantizado para la doble vía río seco – desaguadero» añadió en horas precedentes tanto el ministro de obras públicas servicios y vivienda edgar montaño y el gobernador de la paz santos quispe se reunieron para dar solución al conflicto las autoridades nacionales y departamentales no se pusieron de acuerdo para financiar la obra en cuestión ninguna de las partes cedió a incrementar el porcentaje para financiar el 100% de la carretera /jdlf/</t>
+          <t xml:space="preserve"> la desescalada de casos persiste en el país al igual que el incremento de pacientes recuperados con 1474 registrados la presente jornada además de no reportarse decesos por el virus en bolivia se registraron 75 casos positivos de coronavirus este domingo según los datos del ministerio de salud y deportes santa cruz reportó 16 la paz 39 cochabamba siete chuquisaca dos tarija uno potosí oruro beni y pando ninguno total el país registra hasta el momento un total de 901367 casos positivos de coronavirus de los cuales 831184 son pacientes recuperados el número de decesos se mantienen en 21487 y actualmente hay 48696 casos activos vacunados el reporte de vacunación diario del ministerio de salud detalló que hasta la fecha 6074908 personas recibieron la primera dosis de éstas 4785308 tienen la segunda y 1209248 la tercera además 994961 ciudadanos tienen la vacuna janssen de una sola dosis desde la cartera de salud y deportes anuncian que hasta el domingo se aplicaron 13064425 dosis de las vacunas sputnikv astrazeneca sinopharm pfizer y janssen en todo el territorio nacional</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/25/dan-cuarto-intermedio-al-bloqueo-en-la-ruta-a-desaguadero/</t>
+          <t>https://lapatria.bo/2022/03/27/bolivia-registra-75-nuevos-casos-de-covid-19/</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1544,51 +1544,51 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>e23019b5e8c99dc0c484b712165dc4a7</t>
+          <t>6b48ecd6a319096ec2e8cae0098abbfb</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="G21" t="n">
-        <v>1523</v>
+        <v>1084</v>
       </c>
       <c r="H21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I21" t="n">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>('paz', 4)</t>
+          <t>('salud', 3)</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>('provincia', 3)</t>
+          <t>('hasta', 3)</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>('ingavi', 3)</t>
+          <t>('dosis', 3)</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>embajadores y jefes de misión en bolivia piden a rusia cese de invasión</t>
+          <t>cuatro regiones del país están aisladas por bloqueos</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> a un mes del inicio de las operaciones militares rusas en ucrania diez embajadores y jefes de misión en bolivia se pronunciaron pidiendo el cese a la invasión también condenaron el “demoledor impacto humanitario” producto del conflicto bélico entre ambos países “se cumplen ya cuatro semanas desde que el 24 de febrero rusia invadiera ucrania sin justificación alguna y en violación del derecho internacional sembrando dolor y muerte a su paso desde ese mismo día el agresor ha tenido al frente un pueblo que se defiende valerosamente y no está dispuesto a renunciar a su soberanía y su libertad” se lee en el comunicado el documento lo suscribieron los embajadores de alemania stefan duppel canadá ralph jansen españa javier gassó estados unidos charisse phillips francia hélène roos italia francesco tafuri japón osuma hokida reino unido jeff glekin suecia nicolas weeks y de la unión europea michael dóczy en parte del comunicado señalaron las acciones del presidente ruso vladimir putin como las causantes de la muerte de inocentes también observaron los bombardeos registrados en hospitales escuelas universidades y viviendas incluso rechazaron el ataque indiscriminado a mujeres y niños que huían por corredores humanitarios supuestamente seguros según lo publicado por la agencia de noticias fides anf “el gobierno ruso y sus patrocinadores son responsables de todo ello han violado el derecho internacional y la carta de las naciones unidas ignorando los principios de igualdad soberana de todos los estados de no injerencia en los asuntos internos y la prohibición de recurrir al uso de la fuerza para la solución de controversias con el único objetivo de satisfacer sus intereses particulares” resaltaron los firmantes del documento tras varios meses de tensión entre ambos países europeos el mandatario ruso anunció el inicio de las denominadas “operaciones militares especiales” en ucrania el 24 de febrero los embajadores y los jefes de misiones firmantes del documento también expusieron su preocupación por el futuro no solo de ambos países sino de todas las naciones después de que el conflicto bélico termine “tras esta guerra el mundo no volverá a ser el mismo hay un cambio de escenario para todos pero este momento dramático es perfecto para reafirmar la voluntad de construir un futuro sobre la base de la confianza la justicia los derechos humanos la libertad y la solidaridad es el momento de levantarse contra el autoritarismo y la opresión la fuerza no da la razón nunca lo hizo nunca lo hará” indica el documento en su parte final / lmpt</t>
+          <t xml:space="preserve"> se cumplió una semana desde que se iniciaron los bloqueos en el desaguadero buena vista y en ascensión de guarayos que mantienen aislado parte del eje central del país el gobierno no logra concretar las soluciones necesarias para la resolución de los conflictos y el levantamiento de las medidas de presión la confederación de empresarios privados de bolivia cepb pidió priorizar el diálogo para que se levanten los bloqueos en distintos puntos del país ya que estas medidas de presión solo generan pérdidas económicas cuantiosas “los conflictos sociales que resultan en cierre de carreteras generan pérdidas cuantiosas al transporte comercio e industria y golpean aún más a las empresas ya afectadas por la pandemia y la crisis mundial urge diálogo” fue la petición de los empresarios privados el bloqueo en ascensión de guarayos impide el paso entre santa cruz y beni el de buena vista cerró el flujo vehicular entre santa cruz cochabamba y la paz en el desaguadero el movimiento comercial por la carretera a perú se vio afectado por las medidas de presión en ascensión de guarayos en la comunidad san antonio de la junta el conflicto se debe a que unos comunarios exigen la titulación de un predio incautado hace dos semanas la semana precedente incluso se registraron enfrentamientos entre estas personas y otro grupo que trató de desaojarlos según informó el deber los enfrentamientos dejaron el saldo de una persona fallecida identificada como franklin delgadillo después de este incidente los considerados avasalladores también instalaron un punto de bloqueo exigiendo el arresto de los responsables de esta muerte y que el terreno en cuestión sea adjudicado a su nombre en buena vista son las juntas escolares las que decidieron bloquear la carretera santa cruz cochabamba demandando un bono escolar que fue prometido por el alcalde del lugar pero que no se concretó hasta el momento los intentos de diálogo con ese sector fracasaron y la tensión entre bloqueadores y transportistas afectados creció en la paz comunidades de la provincia de ingavi cumplieron su séptimo día de bloqueos quienes entraron en conflicto por la construcción de la carretera doble vía río secodesaguadero la negativa de la gobernación paceña a pagar el 20 por ciento para la contraparte del proyecto carretero agravó la situación / lmpt</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/26/embajadores-y-jefes-de-mision-en-bolivia-piden-a-rusia-cese-de-invasion/</t>
+          <t>https://lapatria.bo/2022/03/25/cuatro-regiones-del-pais-estan-aisladas-por-bloqueos/</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1598,51 +1598,51 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>7929be2712ef434be43904635ab8aa01</t>
+          <t>e25fd051c1a807a7590167ea247c5ea7</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="G22" t="n">
-        <v>2564</v>
+        <v>2322</v>
       </c>
       <c r="H22" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I22" t="n">
-        <v>241</v>
+        <v>208</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>('documento', 4)</t>
+          <t>('bloqueos', 3)</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>('ucrania', 3)</t>
+          <t>('buena', 3)</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>('embajadores', 3)</t>
+          <t>('vista', 3)</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>santa cruz falta de espacio para neonatos en terapia intensiva de maternidad es crítica hay bebés en sillones</t>
+          <t>dan cuarto intermedio al bloqueo en la ruta a desaguadero</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> el servicio de terapia intensiva para neonatos de la maternidad percy boland en santa cruz está saturado el espacio es tan insuficiente que hasta tres recién nacidos deben compartir una servocuna el director del hospital mario herbas manifestó su preocupación por la situación que consideró como una emergencia pues pueden desatarse brotes de infecciones en los bebés lo que representaría una responsabilidad médicolegal para todo su equipo desde la gobernación de ese departamento informaron que 17 recién nacidos ya fueron trasladados a otros centros médicos de segundo nivel sin embargo esta medida es solo paliativa pues a criterio de herbas lo que se necesita es un nuevo hospital materno infantil reportó el diario el deber la jornada precedente el secretario de salud fernando pacheco solicitó al ministerio de salud la firma de un convenio que permita a los centros médicos privados dar atenciones del sistema único de salud sus especialmente a los bebés que requieren terapia intensiva los médicos que trabajan en la maternidad percy boland lamentaron que los recién nacidos deban compartir las servocunas pues no cuentan con el espacio ni los recursos necesarios para brindarles la atención que requieren un bebé que entra a terapia intensiva neonatal es prematuro requiere un tratamiento cuidadoso sin embargo debe compartir el espacio con al menos otros dos pacientes que un recién nacido comparta la cervocuna es potencialmente peligroso pues otra de las razones por las que los bebés requieren cuidados intensivos son las defensas bajas lo que los vuelve mucho más propensos a contraer cualquier infección los pacientes que salen de terapia intensiva y necesitan cuidados intermedios tampoco tienen un espacio al cual llegar es por eso que el hospital tubo que habilitar incluso sillones para atender a los recién nacidos que lo requieren debido a la precariedad y la falta de espacio en el centro de salud el personal médico debe redoblar sus esfuerzos para atender a los pacientes pues al tratarse de recién nacidos requieren de cuidados muy delicados como ayuda para respirar / lmpt</t>
+          <t xml:space="preserve"> dirigentes de la provincia ingavi anunciaron un cuarto intermedio de 15 días en los bloqueos en la ruta a desaguadero pese a que no se llegó a un acuerdo entre el gobierno y la gobernación de la paz la medida de presión ocasionó que cientos de camiones de carga internacional tanto de bolivia como de perú se vean perjudicados en el comercio de exportación e importación reportó la red erbol  la secretaria ejecutiva de la provincia ingavi maría eugenia millares hizo el anuncio en declaraciones a los medios durante una vigilia en el centro de la ciudad de la paz «se levanta el bloqueo damos un cuarto intermedio de 15 días» manifestóaceptan postura del gobierno y de la gobernación paceña amismo resaltó que los comunarios de la provincia ingavi aceptaron el compromiso de financiamiento del 80% por parte del gobierno y del 10% por parte de la gobernación de la paz para la construcción de la doble vía rio seco – desaguadero respecto al 10% restante indicó que evaluarán la forma de buscar de algún lado el financiamiento“nos sentimos ganadores porque no teníamos ni un 5% garantizado para la doble vía río seco – desaguadero» añadió en horas precedentes tanto el ministro de obras públicas servicios y vivienda edgar montaño y el gobernador de la paz santos quispe se reunieron para dar solución al conflicto las autoridades nacionales y departamentales no se pusieron de acuerdo para financiar la obra en cuestión ninguna de las partes cedió a incrementar el porcentaje para financiar el 100% de la carretera /jdlf/</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/26/santa-cruz-falta-de-espacio-para-neonatos-en-terapia-intensiva-de-maternidad-es-critica-hay-bebes-en-sillones/</t>
+          <t>https://lapatria.bo/2022/03/25/dan-cuarto-intermedio-al-bloqueo-en-la-ruta-a-desaguadero/</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1652,51 +1652,51 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>3f1e863fb92161ecd3c6abe033120f02</t>
+          <t>e23019b5e8c99dc0c484b712165dc4a7</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="G23" t="n">
-        <v>2100</v>
+        <v>1523</v>
       </c>
       <c r="H23" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="I23" t="n">
-        <v>197</v>
+        <v>140</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>('recién', 6)</t>
+          <t>('paz', 4)</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>('espacio', 5)</t>
+          <t>('provincia', 3)</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>('nacidos', 5)</t>
+          <t>('ingavi', 3)</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>aduana extiende horario de atención a operadores hasta las 0300 horas en desaguadero</t>
+          <t>rally vuelta a marbán aprehenden a corredor que atropelló a un menor</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> el horario de atención a operadores en el sector de desaguadero se extiende hasta las tres de la madrugada del domingo para facilitar la importación y exportación de mercancía en esta ruta y facilitar el flujo vehicular esta determinación se logró gracias a las gestiones realizadas por la presidente ejecutiva de la aduana nacional an karina serrudo miranda juntamente el superintendente nacional de aduanas de perú luis enrique vera castillo las entidades que decidieron sumarse a la ampliación de horario son el servicio nacional de sanidad agropecuaria e inocuidad alimentaria senasag la dirección general de migración la superintendencia nacional de aduanas y de administración tributaria sunat de perú y el centro binacional de atención en frontera cebaf de perú informaron desde la institución aduanera hasta el medio día de la presente jornada la an registró el ingreso de 463 camiones a territorio boliviano con mercancía de exportación en horas de la tarde el proceso de exportación se agilizó un total de 436 camiones de carga ingresaron con normalidad a perú durante las siguientes horas continuarán los turnos para el ingreso y la salida del transporte pesado en la ruta con la finalidad de evitar el congestionamiento y acelerar los procesos tanto de la aduana boliviana como la de su par peruana la an calificó como un éxito las labores logísticas gestionadas pues el descongestionamiento en la carretera desaguadero es evidente en tanto el tránsito de los motorizados de comercio exterior se restableció los resultados de la extensión de horario serán evaluados el domingo de acuerdo a la cantidad de motorizados que continúen a la espera de pasar la frontera entre bolivia y perú con base en ese dato se determinará sí es necesario ampliar la extensión de horario por más días el congestionamiento del flujo vehicular en ese sector se debió a un bloqueo instalado por los comunarios de la provincia ingavi quienes mantuvieron la medida de presión por ocho días continuos exigiendo la construcción de la carretera doble vía río secodesaguadero / lmpt</t>
+          <t xml:space="preserve"> el motociclista que atropelló a un menor de edad en el rally vuelta a marbán fue aprehendido informó el director de tránsito del beni coronel marcos céspedes el conductor fue identificado como antonio chemo cuellar de 33 años de edad arrolló al menor la tarde de este domingo cuando cruzaba la ruta del rally en la población de sachojere la competencia fue organizada por novena vez por la asociación beniana de motociclismo y sus representantes aseguraron que están al pendiente del estado de salud tanto del menor como del motociclista céspedes detalló que el conductor sufrió un tec leve y fractura de falange de tercer grado en la mano derecha y está internado en una clínica privada reportó la red erbol “él chemo también se encuentra internado pero además se encuentra aprehendido por disposición del ministerio público” señaló el diagnóstico del menor es reservado sin embargo se conoce que fue intervenido quirúrgicamente en el hospital obrero sufrió un fuerte golpe en la cabeza y tiene una de sus piernas fracturadas el caso fue clasificado por la dirección de tránsito como atropello a peatón en competencia deportiva “sí se debe investigar porque hay lesiones gravísimas o graves y obviamente en el transcurso de la investigación se van a determinar las situaciones que se vayan a seguir posteriormente no porque nosotros hayamos visto que no hay responsabilidad se va a dejar de investigar se tiene que investigar y si el caso amerita obviamente se va a archivar y se va a rechazar” manifestó el coronel /jdlf/</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/26/aduana-extiende-horario-de-atencion-a-operadores-hasta-las-0300-horas-en-desaguadero/</t>
+          <t>https://lapatria.bo/2022/03/21/rally-vuelta-a-marban-aprehenden-a-corredor-que-atropello-a-un-menor/</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1706,51 +1706,51 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>abb876b15918cd2a472317f5c1e903a1</t>
+          <t>38627075644f3e58c9cf8ae402d5652e</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="G24" t="n">
-        <v>2067</v>
+        <v>1524</v>
       </c>
       <c r="H24" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I24" t="n">
-        <v>187</v>
+        <v>134</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>('perú', 5)</t>
+          <t>('menor', 4)</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>('horario', 4)</t>
+          <t>('investigar', 3)</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>('nacional', 4)</t>
+          <t>('motociclista', 2)</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>covid19 en oruro se detectan dos nuevos casos no se reportan decesos</t>
+          <t>rusia da por concluida la “primera fase” de la invasión a ucrania</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> la jornada del 26 de marzo oruro mostró de nuevo una cifra mínima de casos positivos de coronavirus dos en total la tendencia de cero decesos también continuó se cumplieron 18 días sin reportar fallecidos por el virus el reporte del servicio departamental de salud sedes señaló que los dos casos confirmados corresponden al municipio de oruro al igual que las tres personas recuperadas que figuran en el reporte además se descartaron 266 casos total hasta el momento el departamento de oruro registra un total de 35549 casos positivos de coronavirus y 34136 pacientes recuperados actualmente hay 87 casos activos contagios sumados los contagios de la jornada la capital suma 35549 casos positivos de coronavirus seguida huanuni con 1512 casos callapata 1143 machacamarca 392 caracollo 359 sabaya 288 turco 266 salinas de garci mendoza 238 antequera 218 y eucaliptos con 214 casos curahuara de carangas se mantiene con 196 casos al igual que huari con 185 positivos huachacalla 163 santiago de andamarca 154 pazña 149 corque 133 pampa aullagas 103 el choro 87 quillacas 83 en tanto totora 67 huayllamarca 66 soracachi 56 esmeralda 43 yunguyo de litoral 37 belén de andamarca 28 choquecota 26 cruz de machacamarca 26 escara 23 chipaya 21 coipasa 15 la rivera cinco carangas y todos santos uno recuperados ya son 34136 pacientes recuperados en el municipio de oruro huanuni 1469 challapata 1081 machacamarca 374 caracollo 335 sabaya 284 turco 264 salinas de garci mendoza 233 antequera 212 eucaliptus 202 toledo 201 poopó 194 curahuara de carangas se mantiene con 178 pacientes recuperados huari 177 huachacalla 157 santiago de andamarca 148 pazña 146 corque 131 pampa aullagas 101 el choro 87 quillacas 80 huayllamarca 65 finalmente totora 62 soracachi 55 esmeralda 42 yunguyo de litoral 36 belén de andamarca 28 choquecota 25 cruz de machacamarca 24 escara 23 chipaya 21 coipasa 15 la rivera cinco todos santos uno y finalmente carangas uno</t>
+          <t xml:space="preserve"> rusia dio por concluida la “primera fase” de la invasión a ucrania que comenzó el 24 de febrero el anuncio se tradujo como el reconocimiento de que los objetivos planteados cuando iniciaron las operaciones militares no fueron alcanzados el jefe del principal departamento operativo del estado mayor de las fuerzas armadas de rusia sergey rudskoy dijo la jornada precedente que a un mes de que iniciaron las operaciones militares ahora los esfuerzos se centrarán en conseguir la “liberación total” de la región del donbás al este de ucrania el jefe militar también explicó que se consideraron dos opciones para su “operación especial militar” la primera consistía en abarcar toda ucrania y la segunda se enfocaba solo en el donbás según informó el portal de la bbc rudskoy aseguró que el 93% de luhansk y el 54% de donetsk ambas en la región de donbás están bajo control de las tropas rusas estos dos lugares fueron reconocidos por el presidente ruso vladimir putin como repúblicas independientes las declaraciones de rudskoy publicadas por las agencias de noticias estatales rusas apuntan a una posible reducción de los objetivos de guerra de rusia esto después de que las tropas de ese país encontraran una fuerte resistencia al norte de ucrania y especialmente en kiev la capital lo que marcó un “final exitoso” de la primera fase de las operaciones militares según rudskoy fue la destrucción de gran parte de la fuerza aérea y la armada ucraniana el ministerio de defensa ruso no descartó realizar operaciones militares en las ciudades que fueron bloqueadas además afirmaron que rusia reaccionará inmediatamente ante cualquier movimiento para cerrar el espacio aéreo sobre territorio ucraniano algo que el presidente de ese país volodymyr zelensky sigue pidiendo insistentemente la jornada precedente por segunda vez desde el inicio de la invasión el ministerio de defensa ruso dio un informe sobre las bajas en sus tropas reportaron 1351 soldados muertos y 3825 heridos sin embargo fuentes militares ucranianas afirmaron que al menos 15 mil soldados rusos murieron desde el inicio del conflicto aunque esta cifra podría incluir también heridos la inteligencia estadounidense sugiere una cifra más precisa puede ser solo la mitad de ese número / lmpt</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/26/covid-19-en-oruro-se-detectan-dos-nuevos-casos-no-se-reportan-decesos/</t>
+          <t>https://lapatria.bo/2022/03/26/rusia-da-por-concluida-la-primera-fase-de-la-invasion-a-ucrania/</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1760,51 +1760,51 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>832d0bf674f94b758670c4d51bf045ea</t>
+          <t>bae380998c4b801c18fd320bf4a43cd0</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G25" t="n">
-        <v>1940</v>
+        <v>2254</v>
       </c>
       <c r="H25" t="n">
         <v>7</v>
       </c>
       <c r="I25" t="n">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>('oruro', 4)</t>
+          <t>('militares', 5)</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>('positivos', 4)</t>
+          <t>('rusia', 4)</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>('recuperados', 4)</t>
+          <t>('ucrania', 4)</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>bolivia registra 184 casos positivos de covid19</t>
+          <t>ine denuncia desestabilización y politización del censo en santa cruz</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> la desescalada de casos persiste en el país al igual que el incremento de pacientes recuperados con 1963 registrados la presente jornada además de no reportarse decesos por el virus en bolivia se registraron 184 casos positivos de coronavirus este sábado según los datos del ministerio de salud y deportes santa cruz 33 cochabamba 18 la paz 107 chuquisaca cinco tarija uno potosí 18 oruro dos beni ninguno y pando ninguno total el país registra hasta el momento un total de 901292 casos positivos de coronavirus de los cuales 829710 son pacientes recuperados el número de decesos asciende a 21487 y actualmente hay 50095 casos activos vacunados el reporte de vacunación diario del ministerio de salud detalla que hasta la fecha 6074507 personas recibieron la primera dosis de éstas 4784783 tienen la segunda y 1208408 la tercera además 994961 ciudadanos cuentan con la vacuna janssen de una sola dosis desde la cartera de salud y deportes anuncian que hasta el sábado se aplicaron 13062659 dosis de las vacunas sputnikv astrazeneca sinopharm pfizer y janssen en todo el territorio nacional</t>
+          <t xml:space="preserve"> la denuncia de desestabilización y politización del censo de población y vivienda fue hecha por el director ejecutivo del instituto nacional de estadística ine humberto arandia quien también señaló como uno de los principales responsables al presidente de la asamblea legislativa cruceña zvonko matkovic “hay intereses que quieren politizar un proceso que es meramente técnico se quiso hacer ver que no invitamos a la gobernación cruceña a participar de la socialización totalmente falso en el caso de santa cruz participaron el rector de la universidad gabriel rené moreno vicente cuéllar y un exdirector del ine jorge akamine por lo que esta convocatoria fue abierta” afirmó arandia lamentó que haya un “doble discurso” por el rector de la casa superior de estudios cruceña pues en primera instancia ponderó las tareas previas al censo sin embargo dijo otra cosa después también reclamó por las declaraciones y acciones de zvonko matkovic “hace unas semanas el presidente de la asamblea legislativa departamental zvonko matkovic se hizo presente en las puertas del ine indicando que el director no lo quería recibir pero lo que nunca dijo después es que un día antes había recibido una carta por mi persona indicando que se le pedía otro día y el señor matkovic cumpliendo su función política declaró que el ine no lo quería recibir” declaró el director ejecutivo del ine indicó que el proceso del censo será explicado a la sociedad civil de los nueve departamentos del país y a las instituciones que así lo requieran según informó el portal de noticias innovapress arandia también se refirió a la elaboración de la boleta censal que actualmente está en su etapa preliminar y está siendo trabajada por expertos del país en colaboración con organizaciones internacionales “todos los trabajos que estamos realizando están siendo supervisados y analizados por una comisión internacional de alto nivel conformada por expertos internacionales en la temática censal el objetivo del censo tiene que ser avalado por técnicos de naciones unidas la cepal/celade banco mundial banco interamericano de desarrollo y fonplata” explicó en cuanto al presupuesto para el censo arandia explicó que el ine cuenta con 181 millones bolivianos de los cuales 65 fueron otorgados a través del decreto supremo 4664 y serán destinados a la contratación de consultores para llevar adelante el proceso censal además de otros 116 millones de bolivianos entregados mediante trasferencia presupuestaria por el ministerio de economía y finanzas públicas / lmpt</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/26/bolivia-registra-184-casos-positivos-de-covid-19/</t>
+          <t>https://lapatria.bo/2022/03/27/ine-denuncia-desestabilizacion-y-politizacion-del-censo-en-santa-cruz/</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1814,51 +1814,51 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>0577f82b653a440188bea2ca0351b10d</t>
+          <t>513d38dbc59bb31bc88e3af03a1815e4</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="G26" t="n">
-        <v>1090</v>
+        <v>2531</v>
       </c>
       <c r="H26" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I26" t="n">
-        <v>111</v>
+        <v>234</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>('salud', 3)</t>
+          <t>('ine', 6)</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>('hasta', 3)</t>
+          <t>('censo', 5)</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>('dosis', 3)</t>
+          <t>('arandia', 4)</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>exfuncionario de la cns fue aprehendido por la policía acusado de estafar ofreciendo cargos</t>
+          <t>policía aprehende a vladimir irahola villanueva presunto feminicida de vania</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> un hombre identificado como mauricio p r fue aprehendido por efectivos de la policía boliviana quien es acusado de presuntamente estafar a varias personas ofreciéndoles cargos en la caja nacional de salud cns a cambio de dinero informó el ministro de gobierno eduardo del castillo a los medios de comunicación “el señor oscar u m la señora mayra r c el señor isael g r y el señor josé luis c g habrían denunciado que existiría un exfuncionario de la caja nacional de salud que estaba cobrando distintas cantidades de dinero para incorporarlos y que presten servicios al interior de la caja nacional de salud la policía boliviana realizó el operativo correspondiente logrando la aprehensión de este exfuncionario” informó del castillo el ministro presentó este lunes a mauricio p r quien es exfuncionario de la unidad de recursos humanos de la cns y presuntamente cobraba distintas cantidades de dinero para incorporar a las víctimas a dicha institución durante el operativo policial se secuestraron distintas cantidades de dinero entre dólares y bolivianos además de dos equipos de telefonía móvil y documentación que servirá para el proceso de investigación este ciudadano cobraba entre bs 5000 y 22000 a sus víctimas “le pedimos a todo el pueblo boliviano que acuda a las instancias correspondientes para ver si tenemos sujetos como estos que se quieren aprovechar de la buena fe de las y los ciudadanos bolivianos” aseveró del castillo /hnf/</t>
+          <t xml:space="preserve"> la policía informó que luego de un trabajo investigativo en poblaciones fronterizas del beni se ha logrado aprehender a vladimir irahola villanueva principal acusado del feminicidio de su pareja vania trujillo crimen ocurrido en febrero en la ciudad de la paz “informamos a la población que después de un arduo trabajo investigativo en poblaciones fronterizas del beni nuestros servidores policiales procedieron a la aprehensión de vladimir irahola villanueva principal acusado del feminicidio de su esposa vania trujillo” se lee en el comunicado de la policía en sus redes sociales el caso cobró relevancia después de que la activista maría galindo protestó en el estado mayor y la fiscalía reclamando que se había dejado escapar a vladimir irahola presunto autor del feminicidio de vania trujillo el feminicidio se registró el 18 de febrero según las investigaciones el autor del crimen quiso fingir que la víctima había fallecido por ingerir una sustancia tóxica pero se evidenció que fue estrangulada el padre del presunto feminicida de profesión militar fue aprehendido y enviado a la cárcel acusado de haber ayudado a escapar a su hijo con el pasar de los días las investigaciones se volcaron al beni donde vive un amigo del principal sospechoso quien aparentemente sabía del crimen y cobijó al presunto feminicida por lo cual fue aprehendido vladimir irahola se comunicó con su amigo moisés quien se encontraba en beni y le contó que le quitó la vida a su pareja el amigo le pidió fotos y ambos se enviaron audios “por eso que se llega a estas conversaciones y se tiene la aprehensión de moisés vaquero que sería el amigo a quien denominaba ‘yunta o bro’” afirmo la coordinadora de la fiscalía de la paz nilda calle vania trujillo fue asesinada el 18 de febrero en la zona de bajo san antonio de la ciudad de la paz presuntamente en manos de su concubino vladimir de quien se presume que le puso en la boca un líquido usado para limpiar hornos y de esa forma hacer creer que la joven se suicidó sin embargo tras la autopsia se develó que el deceso fue por estrangulamiento /hnf/</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/21/exfuncionario-de-la-cns-fue-aprehendido-por-la-policia-acusado-de-estafar-ofreciendo-cargos/</t>
+          <t>https://lapatria.bo/2022/03/23/policia-aprehende-a-vladimir-irahola-villanueva-presunto-feminicida-de-vania/</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1868,51 +1868,51 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>ceeb8df104b6ed583966bfc82015fc8c</t>
+          <t>57e927df02d32b98814406604e0e832f</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="G27" t="n">
-        <v>1445</v>
+        <v>2086</v>
       </c>
       <c r="H27" t="n">
         <v>8</v>
       </c>
       <c r="I27" t="n">
-        <v>141</v>
+        <v>197</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>('r', 4)</t>
+          <t>('vladimir', 5)</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>('dinero', 4)</t>
+          <t>('beni', 4)</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>('caja', 3)</t>
+          <t>('irahola', 4)</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>la paz envían a la cárcel a militar acusado de ayudar a escapar a su hijo presunto feminicida de vania</t>
+          <t>embajadores y jefes de misión en bolivia piden a rusia cese de invasión</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> el teniente coronel del ejército iván li padre del presunto feminicida de vania t b fue enviado a la cárcel de san pedro de la ciudad de la paz con detención preventiva mientras duran las investigaciones del caso el plazo de la detención preventiva es de cinco meses mientras se realiza la investigación informó el coronel jhonny vega director de la fuerza especial de lucha contra la violencia felcv “el militar está acusado de autoría mediata en el caso puesto que habría ayudado a la fuga de su hijo” indicó el coronel vega el caso de feminicidio de vania fue registrado el 18 de febrero según la investigación el presunto autor vladimir iv hijo del militar detenido habría dicho que la víctima falleció por ingerir una sustancia tóxica pero se evidenció que fue estrangulada el pasado viernes el militar fue aprehendido y se realizó un allanamiento en su domicilio en la cual se secuestraron dos celulares informó el coronel vega la policía continúa en la búsqueda del prófugo vladimir iv /hnf/</t>
+          <t xml:space="preserve"> a un mes del inicio de las operaciones militares rusas en ucrania diez embajadores y jefes de misión en bolivia se pronunciaron pidiendo el cese a la invasión también condenaron el “demoledor impacto humanitario” producto del conflicto bélico entre ambos países “se cumplen ya cuatro semanas desde que el 24 de febrero rusia invadiera ucrania sin justificación alguna y en violación del derecho internacional sembrando dolor y muerte a su paso desde ese mismo día el agresor ha tenido al frente un pueblo que se defiende valerosamente y no está dispuesto a renunciar a su soberanía y su libertad” se lee en el comunicado el documento lo suscribieron los embajadores de alemania stefan duppel canadá ralph jansen españa javier gassó estados unidos charisse phillips francia hélène roos italia francesco tafuri japón osuma hokida reino unido jeff glekin suecia nicolas weeks y de la unión europea michael dóczy en parte del comunicado señalaron las acciones del presidente ruso vladimir putin como las causantes de la muerte de inocentes también observaron los bombardeos registrados en hospitales escuelas universidades y viviendas incluso rechazaron el ataque indiscriminado a mujeres y niños que huían por corredores humanitarios supuestamente seguros según lo publicado por la agencia de noticias fides anf “el gobierno ruso y sus patrocinadores son responsables de todo ello han violado el derecho internacional y la carta de las naciones unidas ignorando los principios de igualdad soberana de todos los estados de no injerencia en los asuntos internos y la prohibición de recurrir al uso de la fuerza para la solución de controversias con el único objetivo de satisfacer sus intereses particulares” resaltaron los firmantes del documento tras varios meses de tensión entre ambos países europeos el mandatario ruso anunció el inicio de las denominadas “operaciones militares especiales” en ucrania el 24 de febrero los embajadores y los jefes de misiones firmantes del documento también expusieron su preocupación por el futuro no solo de ambos países sino de todas las naciones después de que el conflicto bélico termine “tras esta guerra el mundo no volverá a ser el mismo hay un cambio de escenario para todos pero este momento dramático es perfecto para reafirmar la voluntad de construir un futuro sobre la base de la confianza la justicia los derechos humanos la libertad y la solidaridad es el momento de levantarse contra el autoritarismo y la opresión la fuerza no da la razón nunca lo hizo nunca lo hará” indica el documento en su parte final / lmpt</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/21/la-paz-envian-a-la-carcel-a-militar-acusado-de-ayudar-a-escapar-a-su-hijo-presunto-feminicida-de-vania/</t>
+          <t>https://lapatria.bo/2022/03/26/embajadores-y-jefes-de-mision-en-bolivia-piden-a-rusia-cese-de-invasion/</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1922,51 +1922,51 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>101ab6d3a2944285f73df6c296524788</t>
+          <t>7929be2712ef434be43904635ab8aa01</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="G28" t="n">
-        <v>999</v>
+        <v>2564</v>
       </c>
       <c r="H28" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I28" t="n">
-        <v>101</v>
+        <v>241</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>('coronel', 4)</t>
+          <t>('documento', 4)</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>('caso', 3)</t>
+          <t>('ucrania', 3)</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>('vega', 3)</t>
+          <t>('embajadores', 3)</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>condolencia dr juan carlos espinoza zambrana q e p d</t>
+          <t>coronavirus seis nuevos casos en oruro y tres pacientes recuperados</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> spectrolab oruro se adhiere al dolor que embarga a la familia de nuestra compañera de trabajo y amiga jenny anabel espinoza zambrana por la irreparable pérdida de su hermano nuestro sentido pésame que dios les dé fortaleza y su presencia los llene de paz oruro 25 de marzo del 2022</t>
+          <t xml:space="preserve"> las cifras de covid19 en oruro continúan bajas después del feriado de carnaval este jueves se tuvieron seis nuevos contagios y tres pacientes recuperados además ya son 16 días que no se reportan decesos por esta enfermedad el reporte del servicio departamental de salud sedes indica que tanto los seis casos nuevos como las tres personas recuperadas son del municipio de oruro total hasta el momento en el departamento de oruro se registraron 42268 casos de coronavirus además 40587 pacientes se recuperaron 1594 fallecieron y hay 87 personas que todavía tienen el virus contagios con los nuevos contagios la ciudad capital suma 35543 casos seguida de huanuni con 1521 challapata 1143 machacamarca 392 caracollo 359 sabaya 288 turco 266 salinas de garci mendoza 238 antequera 218 eucaliptus 214 toledo 210 poopó 209 curahuara de carangas 196 huari 185 huachacalla 163 santiago de andamarca 154 pazña 149 corque 133 pampa aullagas 103 el choro 87 quillacas 83 en tanto totora 67 huayllamarca 66 soracachi 56 esmeralda 43 yunguyo de litoral 37 belén de andamarca 28 choquecota 26 cruz de machacamarca 26 escara 23 chipaya 21 coipasa 15 la rivera cinco carangas y todos santos uno recuperados el municipio de oruro acumula 34130 personas recuperadas huanuni 1469 challapata 1081 machacamarca 374 caracollo 335 sabaya 284 turco 264 salinas de garci mendoza 233 antequera 212 eucaliptus 202 toledo 201 poopó 194 curahuara de carangas 178 huari 177 huachacalla 157 santiago de andamarca 148 pazña 146 corque 131 pampa aullagas 101 el choro 87 quillacas 80 huayllamarca 65 finalmente totora 62 soracachi 55 esmeralda 42 yunguyo de litoral 36 belén de andamarca 28 choquecota 25 cruz de machacamarca 24 escara 23 chipaya 21 coipasa 15 la rivera cinco todos santos uno y carangas uno</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/26/condolencia-dr-juan-carlos-espinoza-zambrana-q-e-p-d/</t>
+          <t>https://lapatria.bo/2022/03/25/coronavirus-seis-nuevos-casos-en-oruro-y-tres-pacientes-recuperados/</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1976,51 +1976,51 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>efe86d61b07d57d150fa2fa323238da4</t>
+          <t>36a7cde7d7d990cff2e7a206f6095c19</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="G29" t="n">
-        <v>282</v>
+        <v>1775</v>
       </c>
       <c r="H29" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I29" t="n">
-        <v>31</v>
+        <v>221</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>('oruro', 2)</t>
+          <t>('oruro', 4)</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>('', 1)</t>
+          <t>('machacamarca', 4)</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>('spectrolab', 1)</t>
+          <t>('carangas', 4)</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>gobierno peruano pide a la oea presenciar debate de moción de vacancia de pedro castillo</t>
+          <t>condolencia dr juan carlos espinoza zambrana q e p d</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> desde el gobierno peruano solicitaron la jornada precedente la presencia de funcionarios de la organización de los estados americanos oea para presenciar el debate de moción de vacancia del presidente pedro castillo el congreso escuchará el 28 de marzo la defensa del mandatario para tratar el tema de su destitución en una misiva enviada por el canciller césar landa a la presidenta del congreso maría carmen alva se solicitó que se acepte la presencia de testigos de la oea con el motivo de que el debate se desarrolle con trasparencia ante la ciudadanía y la comunidad internacional en la carta se expresó la importancia de este acontecimiento pues para landa depende de este proceso la gobernabilidad de perú y la vigencia de la democracia no solo en ese país sino en todo el continente el canciller pidió la presencia de tres funcionarios específicos de la oea para que presencien el debate en el pleno del congreso el representante de ese ente en el perú miguel ángel trinidad el secretario de asuntos jurídicos jean miguel arrighi y la secretaria de acceso a derechos y equidad maricarmen plata el partido opositor “avanza país” cuestionó esta petición a la presidencia del congreso pues consideraron que no hay precedentes para incluir a la oea como veedores en un proceso como la vacancia según informó el portal de noticias deutsche welle por su parte el primer ministro aníbal torres destacó el pronunciamiento de la comisión interamericana de derechos humanos cidh quienes expresaron el viernes reciente su preocupación por la situación política en perú y el impacto que podría tener en los derechos humanos «la vacancia presidencial debe llevarse a cabo conforme al debido proceso constitucional y fundarse en conductas señaladas con precisión que doten a este proceso de objetividad imparcialidad y garantías del debido proceso a fin de asegurar que sea un recurso que no se use para afectar el orden democrático constituido y los derechos políticos de los y las peruanas» informó la comisión en un comunicado el lunes 28 de marzo el congreso escuchará la defensa de pedro castillo ante la acusación por una supuesta «incapacidad moral permanente» posteriormente se votará el pedido de destitución presentado por varios grupos de ultraderecha que aparentemente no cuentan con los 87 votos necesarios para hacer a abandonar el cargo al presidente / lmpt</t>
+          <t xml:space="preserve"> spectrolab oruro se adhiere al dolor que embarga a la familia de nuestra compañera de trabajo y amiga jenny anabel espinoza zambrana por la irreparable pérdida de su hermano nuestro sentido pésame que dios les dé fortaleza y su presencia los llene de paz oruro 25 de marzo del 2022</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/26/gobierno-peruano-pide-a-la-oea-presenciar-debate-de-mocion-de-vacancia-de-pedro-castillo/</t>
+          <t>https://lapatria.bo/2022/03/26/condolencia-dr-juan-carlos-espinoza-zambrana-q-e-p-d/</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2030,51 +2030,51 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>4c8b311107f359a09f787328ed22add5</t>
+          <t>efe86d61b07d57d150fa2fa323238da4</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="G30" t="n">
-        <v>2367</v>
+        <v>282</v>
       </c>
       <c r="H30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I30" t="n">
-        <v>209</v>
+        <v>31</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>('congreso', 5)</t>
+          <t>('oruro', 2)</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>('proceso', 5)</t>
+          <t>('', 1)</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>('oea', 4)</t>
+          <t>('spectrolab', 1)</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>el salvador declara estado de excepción ante la escalada criminal</t>
+          <t>concluyen obras de readecuación en el hospital obrero de la cns</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> la asamblea legislativa de el salvador decretó la madrugada de este domingo un régimen de excepción a raíz de un “incremento desmedido” de los homicidios la muerte de 76 personas en dos días un récord en la historia reciente de ese país fueron atribuidas a las pandillas “declárase en todo el territorio nacional régimen de excepción derivado de las graves perturbaciones al orden público por grupos delincuenciales” consignó el decreto aprobado por amplia mayoría en el parlamento el órgano legislativo con 67 votos de los 84 diputados suspendió por 30 días la libertad de asociación derecho de defensa plazo de detención administrativa inviolabilidad de la correspondencia y telecomunicaciones según informó el portal de noticias infobae el gobierno de nayib bukele planteó esta medida al congreso para reducir el repunte de la delincuencia y establecer la paz puesto que consideraron que el salvador vive perturbaciones graves del orden público a raíz de la delincuencia la carta magna salvadoreña estipula que la suspensión de garantías constitucionales se puede dar en los siguientes casos “guerra invasión del territorio rebelión sedición catástrofe epidemia u otra calamidad general o de graves perturbaciones del orden público” al invocar este artículo de la constitución el congreso puede suspender la libertad de entrada y salida del país la libertad de expresión la inviolabilidad de la correspondencia y la prohibición de la intervención de telecomunicaciones sin orden judicial también figuran la libertad de asociación el derecho de todo detenido a ser informado de las razones de su arresto la garantía de la asistencia de un defensor en los procesos judiciales y el plazo máximo de 72 horas de detención administrativa y consignación ante un juez con los homicidios registrados hasta el viernes el salvador alcanzó los 86 homicidios en marzo según datos de la policía cifra superior a las que se registraron en enero y febrero con 85 y 79 muertes violentas respectivamente en noviembre de 2021 el país también registró un alza repentina de los homicidios que dejó más de 40 asesinatos en tres días en ese entonces bukele criticó los señalamientos de que su gobierno tenía una “tregua” con las pandillas / lmpt</t>
+          <t xml:space="preserve"> concluyeron las obras de readecuación de ambientes para residencia médica y readecuación e implementación de baños y duchas en el sótano del hospital de atención integral general haig obrero n° 4 el jueves 24 de marzo se realizó la entrega oficial en los ambientes del nosocomio y con la presencia de autoridades de la caja nacional de salud cns tanto nacionales como regionales además de la asistencia de autoridades departamentales se realizó un emotivo acto de entrega de las obras realizadas el administrador regional de la cns johnny bohórquez velasco indicó que las nuevas dependencias tendrán como principales beneficiarios a los residentes médicos tanto actuales como también de futuras generaciones</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://lapatria.bo/2022/03/27/el-salvador-declara-estado-de-excepcion-ante-la-escalada-criminal/</t>
+          <t>https://lapatria.bo/2022/03/26/concluyen-obras-de-readecuacion-en-el-hospital-obrero-de-la-cns/</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2084,34 +2084,34 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>82d3d677e39b2cf1c78fbdbbcdc84439</t>
+          <t>99786ea273c5645ee5b640ff762c5e73</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G31" t="n">
-        <v>2226</v>
+        <v>708</v>
       </c>
       <c r="H31" t="n">
         <v>6</v>
       </c>
       <c r="I31" t="n">
-        <v>196</v>
+        <v>64</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>('homicidios', 4)</t>
+          <t>('obras', 2)</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>('orden', 4)</t>
+          <t>('readecuación', 2)</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>('libertad', 4)</t>
+          <t>('ambientes', 2)</t>
         </is>
       </c>
     </row>

</xml_diff>